<commit_message>
aggiunti ultimi test case di validazione
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sorgenti\FSE 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B601C0-DA74-4DEC-A6D4-5EBC7345885D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0B397A-AB7D-49D0-AE26-939CB5ADA53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-10860" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="872">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4561,6 +4561,36 @@
     "status": 422,
     "instance": "/validation/error",
     "workflowInstanceId": "2.16.840.1.113883.2.9.2.150.4.4.cce472283545a35052f3f7432f8d1334ac1d01c5c46f5a817ece8668b0083dbc.9457bcc9ed^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"
+}</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.cce472283545a35052f3f7432f8d1334ac1d01c5c46f5a817ece8668b0083dbc.04d30b54a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-30T12:04:11Z</t>
+  </si>
+  <si>
+    <t>cb2c586272462c78</t>
+  </si>
+  <si>
+    <t>e3a5960ecfc7670c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.cce472283545a35052f3f7432f8d1334ac1d01c5c46f5a817ece8668b0083dbc.b0c96c8415^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-29T12:18:00Z</t>
+  </si>
+  <si>
+    <t>{
+    "traceID": "e3a5960ecfc7670c",
+    "spanID": "e3a5960ecfc7670c",
+    "type": "/msg/semantic",
+    "title": "Errore semantico.",
+    "detail": "[ERRORE-b19| L’elemento organizer di tipo 'BATTERY' (@classCode='BATTERY') DEVE contenere l’elemento organizer/code.\n\t\t\t],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ],[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ]",
+    "status": 422,
+    "instance": "/validation/error",
+    "workflowInstanceId": "2.16.840.1.113883.2.9.2.150.4.4.cce472283545a35052f3f7432f8d1334ac1d01c5c46f5a817ece8668b0083dbc.b0c96c8415^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"
 }</t>
   </si>
 </sst>
@@ -4893,7 +4923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4983,6 +5013,21 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5004,24 +5049,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7483,10 +7510,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="R69" sqref="R69"/>
+      <selection pane="bottomRight" activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -7528,14 +7555,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42" t="s">
         <v>842</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7553,14 +7580,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>830</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7578,12 +7605,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>831</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7602,12 +7629,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>832</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7625,8 +7652,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -7891,11 +7918,21 @@
       <c r="E13" s="22" t="s">
         <v>412</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="F13" s="23">
+        <v>45015</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>866</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>867</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>865</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>489</v>
+      </c>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -8663,11 +8700,11 @@
       </c>
       <c r="J35" s="25"/>
       <c r="K35" s="25"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="45" t="s">
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34"/>
+      <c r="P35" s="33" t="s">
         <v>859</v>
       </c>
       <c r="Q35" s="25"/>
@@ -8945,11 +8982,11 @@
       </c>
       <c r="J43" s="25"/>
       <c r="K43" s="25"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="47"/>
-      <c r="N43" s="47"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="45" t="s">
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="34"/>
+      <c r="P43" s="33" t="s">
         <v>859</v>
       </c>
       <c r="Q43" s="25"/>
@@ -9213,7 +9250,7 @@
       <c r="E51" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="F51" s="48">
+      <c r="F51" s="35">
         <v>45014</v>
       </c>
       <c r="G51" s="24"/>
@@ -9225,7 +9262,7 @@
       <c r="M51" s="25"/>
       <c r="N51" s="25"/>
       <c r="O51" s="25"/>
-      <c r="P51" s="45" t="s">
+      <c r="P51" s="33" t="s">
         <v>859</v>
       </c>
       <c r="Q51" s="25"/>
@@ -9624,7 +9661,7 @@
       <c r="J62" s="25" t="s">
         <v>829</v>
       </c>
-      <c r="K62" s="45" t="s">
+      <c r="K62" s="33" t="s">
         <v>850</v>
       </c>
       <c r="L62" s="25"/>
@@ -9662,7 +9699,7 @@
       <c r="J63" s="25" t="s">
         <v>829</v>
       </c>
-      <c r="K63" s="45" t="s">
+      <c r="K63" s="33" t="s">
         <v>851</v>
       </c>
       <c r="L63" s="25"/>
@@ -9735,10 +9772,10 @@
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
       <c r="I65" s="24"/>
-      <c r="J65" s="45" t="s">
+      <c r="J65" s="33" t="s">
         <v>829</v>
       </c>
-      <c r="K65" s="45" t="s">
+      <c r="K65" s="33" t="s">
         <v>860</v>
       </c>
       <c r="L65" s="25"/>
@@ -9810,7 +9847,7 @@
       <c r="F67" s="23">
         <v>45014</v>
       </c>
-      <c r="G67" s="49" t="s">
+      <c r="G67" s="36" t="s">
         <v>862</v>
       </c>
       <c r="H67" s="24" t="s">
@@ -9819,7 +9856,7 @@
       <c r="I67" s="24" t="s">
         <v>863</v>
       </c>
-      <c r="J67" s="45"/>
+      <c r="J67" s="33"/>
       <c r="K67" s="25"/>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
@@ -9828,7 +9865,7 @@
       <c r="P67" s="25"/>
       <c r="Q67" s="25"/>
       <c r="R67" s="26"/>
-      <c r="S67" s="50" t="s">
+      <c r="S67" s="37" t="s">
         <v>864</v>
       </c>
       <c r="T67" s="28" t="s">
@@ -9855,10 +9892,10 @@
       <c r="G68" s="24"/>
       <c r="H68" s="24"/>
       <c r="I68" s="24"/>
-      <c r="J68" s="46" t="s">
+      <c r="J68" s="25" t="s">
         <v>829</v>
       </c>
-      <c r="K68" s="46" t="s">
+      <c r="K68" s="25" t="s">
         <v>853</v>
       </c>
       <c r="L68" s="25"/>
@@ -9873,7 +9910,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="159" thickBot="1">
+    <row r="69" spans="1:20" ht="409.6" thickBot="1">
       <c r="A69" s="20">
         <v>62</v>
       </c>
@@ -9889,12 +9926,20 @@
       <c r="E69" s="22" t="s">
         <v>518</v>
       </c>
-      <c r="F69" s="23"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="24"/>
-      <c r="J69" s="46"/>
-      <c r="K69" s="46"/>
+      <c r="F69" s="23">
+        <v>45015</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>870</v>
+      </c>
+      <c r="H69" s="24" t="s">
+        <v>868</v>
+      </c>
+      <c r="I69" s="24" t="s">
+        <v>869</v>
+      </c>
+      <c r="J69" s="25"/>
+      <c r="K69" s="25"/>
       <c r="L69" s="25"/>
       <c r="M69" s="25"/>
       <c r="N69" s="25"/>
@@ -9902,7 +9947,9 @@
       <c r="P69" s="25"/>
       <c r="Q69" s="25"/>
       <c r="R69" s="26"/>
-      <c r="S69" s="27"/>
+      <c r="S69" s="27" t="s">
+        <v>871</v>
+      </c>
       <c r="T69" s="28" t="s">
         <v>51</v>
       </c>
@@ -20243,7 +20290,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="201.6" hidden="1">
+    <row r="374" spans="1:20" ht="244.8" hidden="1">
       <c r="A374" s="20">
         <v>367</v>
       </c>

</xml_diff>

<commit_message>
aggiunti i test case di radiologia
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sorgenti\FSE 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9136B4D0-32BD-4EAA-9D54-739531021F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3114A2B0-1EA5-43FA-AC78-117AA3DB1C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10860" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Summary!$A$1:$D$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$55</definedName>
     <definedName name="filtro" localSheetId="2">TestCases!$A$9:$S$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="263">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -365,6 +365,38 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Laboratorio dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 5" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LAB_KO</t>
@@ -412,6 +444,9 @@
     </r>
   </si>
   <si>
+    <t>VALIDAZIONE_TOKEN_JWT_RAD_KO</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO</t>
   </si>
   <si>
@@ -457,6 +492,9 @@
     </r>
   </si>
   <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_LAB_TIMEOUT</t>
   </si>
   <si>
@@ -467,6 +505,9 @@
     <t>SI</t>
   </si>
   <si>
+    <t>VALIDAZIONE_RAD_TIMEOUT</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT6_KO</t>
   </si>
   <si>
@@ -542,6 +583,152 @@
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation"al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT5_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT7_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT8_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT11_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.  
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT13_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT14_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT15_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT17_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT18_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT19_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT20_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT21_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT22_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RAD_CT23_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
@@ -867,12 +1054,177 @@
   <si>
     <t>L'operatore deve correggere la configurazione dell'esame e rigenerare il CDA2</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Precondizioni:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Il fornitore utilizza un token jwt mancante di campi obbligatori, quindi non valido.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Al fine di rendere non valido il token è necessario non valorizzare nel JWT il campo "purpose_of_use".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Precondizioni:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Il fornitore utilizza un token jwt con dei campi valorizzati in maniera errata.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Al fine di rendere non valido il token è necessario valorizzare il campo "action_id" con la stringa "TEST" (valore non ammesso).</t>
+    </r>
+  </si>
+  <si>
+    <t>Il sistema invia i dati al fascicolo sanitario solo all'effettiva presenza di un refferto</t>
+  </si>
+  <si>
+    <t>3ecce8c95eae312d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.75cc2b4498^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T11:52:41Z</t>
+  </si>
+  <si>
+    <t>Il dato opzionale non è gestito dall'applicativo, il medico può eventualmente inserire la conclusione all'interno del testo del referto</t>
+  </si>
+  <si>
+    <t>Le sezioni opzionali:  
+1. Conclusione;
+2. Suggerimenti per il medico prescrittore;
+3. DICOM Object Catalog
+non sono gestite dal nostro applicativo</t>
+  </si>
+  <si>
+    <t>Il sistema non prevede la gestione della sezione richiesta</t>
+  </si>
+  <si>
+    <t>Il sistema non accetta valori diversi da quelli ammessi: ‘Accesso Programmato’, ’Accesso Diretto’, ’Accesso Programmato Radiologia’, ‘Accesso Diretto Radiologia'</t>
+  </si>
+  <si>
+    <t>73080d6203fbadb5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.9fc53d6cd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-05T16:45:36Z</t>
+  </si>
+  <si>
+    <t>{
+    "traceID": "73080d6203fbadb5",
+    "spanID": "73080d6203fbadb5",
+    "type": "/msg/syntax",
+    "title": "Errore di sintassi.",
+    "detail": "ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.",
+    "status": 400,
+    "instance": "/validation/error",
+    "workflowInstanceId": "2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.9fc53d6cd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"
+}</t>
+  </si>
+  <si>
+    <t>597ffaba02e8b492</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.72927043bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T10:43:13Z</t>
+  </si>
+  <si>
+    <t>{
+    "traceID": "597ffaba02e8b492",
+    "spanID": "597ffaba02e8b492",
+    "type": "/msg/syntax",
+    "title": "Errore di sintassi.",
+"detail": "ERROR: -1,-1 cvc-enumeration-valid: Value 'TEST' is not facet-valid with respect to enumeration '[AFFL, AGNT, ASSIGNED, COMPAR, SGNOFF, CON, ECON, NOK, GUARD, CIT, COVPTY, CLAIM, NAMED, DEPEN, INDIV, SUBSCR, PROG, CRINV, CRSPNSR, EMP, MIL, GUAR, INVSBJ, CASEBJ, RESBJ, LIC, NOT, PROV, PAT, PAYEE, PAYOR, POLHOLD, QUAL, SPNSR, STD, UNDWRT, CAREGIVER, PRS, ACCESS, ADJY, CONC, BOND, CONY, ADMM, BIRTHPL, DEATHPLC, DST, RET, EXPR, HLD, HLTHCHRT, IDENT, MANU, THER, MNT, OWN, RGPR, SDLOC, DSDLOC, ISDLOC, TERR, USED, WRTE]'. It must be a value from the enumeration.,ERROR: -1,-1 cvc-attribute.3: The value 'TEST' of attribute 'classCode' on element 'associatedEntity' is not valid with respect to its type, 'RoleClassAssociative'.",
+    "status": 400,
+    "instance": "/validation/error",
+    "workflowInstanceId": "2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.72927043bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"
+}</t>
+  </si>
+  <si>
+    <t>L'operatore deve correggere la configurazione della tipologia di utente e rigenerare il CDA2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -933,6 +1285,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1197,7 +1557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1302,6 +1662,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1324,10 +1699,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3789,10 +4167,10 @@
   <dimension ref="A1:T607"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
+      <selection pane="bottomRight" activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3800,7 +4178,7 @@
     <col min="1" max="1" width="6.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" customWidth="1"/>
     <col min="5" max="5" width="74.44140625" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
     <col min="7" max="7" width="22.21875" customWidth="1"/>
@@ -3834,14 +4212,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="41"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="46"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3859,14 +4237,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="41"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="54" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="46"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3884,12 +4262,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="41"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="46"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3908,12 +4286,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="41"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="46"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3931,8 +4309,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4049,7 +4427,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="202.2" thickBot="1">
+    <row r="10" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A10" s="20">
         <v>1</v>
       </c>
@@ -4069,16 +4447,16 @@
         <v>45014</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
@@ -4093,7 +4471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="202.2" thickBot="1">
+    <row r="11" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A11" s="20">
         <v>2</v>
       </c>
@@ -4113,16 +4491,16 @@
         <v>45014</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
@@ -4137,7 +4515,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="202.2" thickBot="1">
+    <row r="12" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A12" s="20">
         <v>3</v>
       </c>
@@ -4157,16 +4535,16 @@
         <v>45014</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>158</v>
+        <v>207</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
@@ -4181,7 +4559,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="202.2" thickBot="1">
+    <row r="13" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A13" s="20">
         <v>4</v>
       </c>
@@ -4201,16 +4579,16 @@
         <v>45015</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>186</v>
+        <v>235</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
@@ -4225,7 +4603,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="202.2" thickBot="1">
+    <row r="14" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A14" s="20">
         <v>5</v>
       </c>
@@ -4245,16 +4623,16 @@
         <v>45014</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
@@ -4269,7 +4647,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="187.8" thickBot="1">
+    <row r="15" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A15" s="20">
         <v>28</v>
       </c>
@@ -4280,41 +4658,41 @@
         <v>44</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F15" s="23">
         <v>45014</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K15" s="25"/>
       <c r="L15" s="34" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="M15" s="34" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="O15" s="34" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="P15" s="33" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
@@ -4323,7 +4701,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="173.4" thickBot="1">
+    <row r="16" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A16" s="20">
         <v>36</v>
       </c>
@@ -4334,41 +4712,41 @@
         <v>44</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="F16" s="23">
         <v>45014</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="34" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="M16" s="34" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4377,7 +4755,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="72.599999999999994" thickBot="1">
+    <row r="17" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A17" s="20">
         <v>44</v>
       </c>
@@ -4388,10 +4766,10 @@
         <v>44</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F17" s="35">
         <v>45014</v>
@@ -4406,7 +4784,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="33" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4415,7 +4793,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="159" thickBot="1">
+    <row r="18" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A18" s="20">
         <v>52</v>
       </c>
@@ -4426,20 +4804,20 @@
         <v>44</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -4453,7 +4831,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="159" thickBot="1">
+    <row r="19" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A19" s="20">
         <v>53</v>
       </c>
@@ -4464,20 +4842,20 @@
         <v>44</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
@@ -4491,7 +4869,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="159" thickBot="1">
+    <row r="20" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A20" s="20">
         <v>54</v>
       </c>
@@ -4502,20 +4880,20 @@
         <v>44</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
       <c r="J20" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -4529,7 +4907,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="159" thickBot="1">
+    <row r="21" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A21" s="20">
         <v>55</v>
       </c>
@@ -4540,20 +4918,20 @@
         <v>44</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="F21" s="23"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
       <c r="J21" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -4567,7 +4945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="159" thickBot="1">
+    <row r="22" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A22" s="20">
         <v>56</v>
       </c>
@@ -4578,20 +4956,20 @@
         <v>44</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
       <c r="J22" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -4605,7 +4983,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="159" thickBot="1">
+    <row r="23" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A23" s="20">
         <v>57</v>
       </c>
@@ -4616,20 +4994,20 @@
         <v>44</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
       <c r="J23" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -4643,7 +5021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="159" thickBot="1">
+    <row r="24" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A24" s="20">
         <v>58</v>
       </c>
@@ -4654,20 +5032,20 @@
         <v>44</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
       <c r="J24" s="33" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -4681,7 +5059,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="159" thickBot="1">
+    <row r="25" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A25" s="20">
         <v>59</v>
       </c>
@@ -4692,20 +5070,20 @@
         <v>44</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -4719,7 +5097,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="409.6" thickBot="1">
+    <row r="26" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A26" s="20">
         <v>60</v>
       </c>
@@ -4730,52 +5108,52 @@
         <v>44</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="F26" s="23">
         <v>45014</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>181</v>
+        <v>230</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>180</v>
+        <v>229</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>182</v>
+        <v>231</v>
       </c>
       <c r="J26" s="33" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K26" s="25"/>
       <c r="L26" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="P26" s="33" t="s">
-        <v>194</v>
+        <v>243</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
       <c r="S26" s="37" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="159" thickBot="1">
+    <row r="27" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A27" s="20">
         <v>61</v>
       </c>
@@ -4786,20 +5164,20 @@
         <v>44</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
       <c r="I27" s="24"/>
       <c r="J27" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
@@ -4813,7 +5191,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="409.6" thickBot="1">
+    <row r="28" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A28" s="20">
         <v>62</v>
       </c>
@@ -4824,52 +5202,52 @@
         <v>44</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F28" s="23">
         <v>45015</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>189</v>
+        <v>238</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>188</v>
+        <v>237</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K28" s="25"/>
       <c r="L28" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="M28" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>194</v>
+        <v>243</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="26"/>
       <c r="S28" s="27" t="s">
-        <v>190</v>
+        <v>239</v>
       </c>
       <c r="T28" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="201.6">
+    <row r="29" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A29" s="20">
         <v>191</v>
       </c>
@@ -4879,26 +5257,26 @@
       <c r="C29" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="51" t="s">
-        <v>95</v>
+      <c r="D29" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>144</v>
       </c>
       <c r="F29" s="23">
         <v>45014</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K29" s="25"/>
       <c r="L29" s="25"/>
@@ -4913,449 +5291,1069 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="15"/>
-    </row>
-    <row r="31" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="15"/>
-    </row>
-    <row r="32" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="15"/>
-    </row>
-    <row r="33" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="15"/>
-    </row>
-    <row r="34" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="15"/>
-    </row>
-    <row r="35" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="15"/>
-    </row>
-    <row r="36" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="15"/>
-    </row>
-    <row r="37" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="15"/>
-    </row>
-    <row r="38" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="13"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="15"/>
-    </row>
-    <row r="39" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="13"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="15"/>
-    </row>
-    <row r="40" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="15"/>
-    </row>
-    <row r="41" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="15"/>
-    </row>
-    <row r="42" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="15"/>
-    </row>
-    <row r="43" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="15"/>
-    </row>
-    <row r="44" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="15"/>
-    </row>
-    <row r="45" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="15"/>
-    </row>
-    <row r="46" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="15"/>
-    </row>
-    <row r="47" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="13"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="15"/>
-    </row>
-    <row r="48" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="13"/>
-      <c r="Q48" s="13"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="15"/>
-    </row>
-    <row r="49" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="13"/>
-      <c r="P49" s="13"/>
-      <c r="Q49" s="13"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="15"/>
-    </row>
-    <row r="50" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="15"/>
-    </row>
-    <row r="51" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="13"/>
-      <c r="P51" s="13"/>
-      <c r="Q51" s="13"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="15"/>
-    </row>
-    <row r="52" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="13"/>
-      <c r="O52" s="13"/>
-      <c r="P52" s="13"/>
-      <c r="Q52" s="13"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="15"/>
-    </row>
-    <row r="53" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="14"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="15"/>
-    </row>
-    <row r="54" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
-      <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="13"/>
-      <c r="O54" s="13"/>
-      <c r="P54" s="13"/>
-      <c r="Q54" s="13"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="2"/>
-      <c r="T54" s="15"/>
-    </row>
-    <row r="55" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="13"/>
-      <c r="O55" s="13"/>
-      <c r="P55" s="13"/>
-      <c r="Q55" s="13"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="2"/>
-      <c r="T55" s="15"/>
-    </row>
-    <row r="56" spans="6:20" ht="14.25" customHeight="1">
+    <row r="30" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A30" s="40">
+        <v>11</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="35">
+        <v>45020</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="H30" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="J30" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A31" s="40">
+        <v>12</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K31" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A32" s="40">
+        <v>13</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K32" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A33" s="40">
+        <v>14</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="35"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K33" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="37"/>
+      <c r="T33" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A34" s="40">
+        <v>31</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="F34" s="23">
+        <v>45014</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="I34" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="K34" s="25"/>
+      <c r="L34" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="M34" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="N34" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="O34" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="P34" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A35" s="40">
+        <v>39</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="F35" s="23">
+        <v>45014</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="K35" s="25"/>
+      <c r="L35" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="M35" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="N35" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="O35" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="P35" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A36" s="40">
+        <v>47</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="35">
+        <v>45014</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A37" s="40">
+        <v>75</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K37" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A38" s="40">
+        <v>76</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A39" s="40">
+        <v>77</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K39" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A40" s="40">
+        <v>78</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K40" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="37"/>
+      <c r="T40" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A41" s="40">
+        <v>79</v>
+      </c>
+      <c r="B41" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K41" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="41"/>
+      <c r="S41" s="37"/>
+      <c r="T41" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A42" s="40">
+        <v>80</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K42" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="37"/>
+      <c r="T42" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A43" s="40">
+        <v>81</v>
+      </c>
+      <c r="B43" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="35">
+        <v>45022</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="I43" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="J43" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="K43" s="33"/>
+      <c r="L43" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="M43" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N43" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="O43" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="41"/>
+      <c r="S43" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="T43" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A44" s="40">
+        <v>82</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K44" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="33"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="41"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A45" s="40">
+        <v>83</v>
+      </c>
+      <c r="B45" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K45" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="33"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="33"/>
+      <c r="Q45" s="33"/>
+      <c r="R45" s="41"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A46" s="40">
+        <v>84</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="35">
+        <v>45021</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="H46" s="55" t="s">
+        <v>254</v>
+      </c>
+      <c r="I46" s="55" t="s">
+        <v>255</v>
+      </c>
+      <c r="J46" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="K46" s="33"/>
+      <c r="L46" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="M46" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N46" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="O46" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="P46" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q46" s="33"/>
+      <c r="R46" s="41"/>
+      <c r="S46" s="57" t="s">
+        <v>257</v>
+      </c>
+      <c r="T46" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A47" s="40">
+        <v>85</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="K47" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="33"/>
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="41"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A48" s="40">
+        <v>86</v>
+      </c>
+      <c r="B48" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K48" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="33"/>
+      <c r="O48" s="33"/>
+      <c r="P48" s="33"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="41"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A49" s="40">
+        <v>87</v>
+      </c>
+      <c r="B49" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K49" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="41"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A50" s="40">
+        <v>88</v>
+      </c>
+      <c r="B50" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K50" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L50" s="33"/>
+      <c r="M50" s="33"/>
+      <c r="N50" s="33"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="41"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A51" s="40">
+        <v>89</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K51" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="33"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="41"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A52" s="40">
+        <v>90</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K52" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+      <c r="N52" s="33"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="33"/>
+      <c r="Q52" s="33"/>
+      <c r="R52" s="41"/>
+      <c r="S52" s="37"/>
+      <c r="T52" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A53" s="40">
+        <v>91</v>
+      </c>
+      <c r="B53" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K53" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="33"/>
+      <c r="P53" s="33"/>
+      <c r="Q53" s="33"/>
+      <c r="R53" s="41"/>
+      <c r="S53" s="37"/>
+      <c r="T53" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+      <c r="A54" s="40">
+        <v>92</v>
+      </c>
+      <c r="B54" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="F54" s="35"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K54" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="33"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="33"/>
+      <c r="Q54" s="33"/>
+      <c r="R54" s="41"/>
+      <c r="S54" s="37"/>
+      <c r="T54" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" ht="34.950000000000003" customHeight="1">
+      <c r="A55" s="40">
+        <v>93</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55" s="35"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="K55" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="N55" s="33"/>
+      <c r="O55" s="33"/>
+      <c r="P55" s="33"/>
+      <c r="Q55" s="33"/>
+      <c r="R55" s="41"/>
+      <c r="S55" s="37"/>
+      <c r="T55" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" ht="14.25" customHeight="1">
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -5372,7 +6370,7 @@
       <c r="S56" s="2"/>
       <c r="T56" s="15"/>
     </row>
-    <row r="57" spans="6:20" ht="14.25" customHeight="1">
+    <row r="57" spans="1:20" ht="14.25" customHeight="1">
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -5389,7 +6387,7 @@
       <c r="S57" s="2"/>
       <c r="T57" s="15"/>
     </row>
-    <row r="58" spans="6:20" ht="14.25" customHeight="1">
+    <row r="58" spans="1:20" ht="14.25" customHeight="1">
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
@@ -5406,7 +6404,7 @@
       <c r="S58" s="2"/>
       <c r="T58" s="15"/>
     </row>
-    <row r="59" spans="6:20" ht="14.25" customHeight="1">
+    <row r="59" spans="1:20" ht="14.25" customHeight="1">
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
@@ -5423,7 +6421,7 @@
       <c r="S59" s="2"/>
       <c r="T59" s="15"/>
     </row>
-    <row r="60" spans="6:20" ht="14.25" customHeight="1">
+    <row r="60" spans="1:20" ht="14.25" customHeight="1">
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -5440,7 +6438,7 @@
       <c r="S60" s="2"/>
       <c r="T60" s="15"/>
     </row>
-    <row r="61" spans="6:20" ht="14.25" customHeight="1">
+    <row r="61" spans="1:20" ht="14.25" customHeight="1">
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
@@ -5457,7 +6455,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="15"/>
     </row>
-    <row r="62" spans="6:20" ht="14.25" customHeight="1">
+    <row r="62" spans="1:20" ht="14.25" customHeight="1">
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
@@ -5474,7 +6472,7 @@
       <c r="S62" s="2"/>
       <c r="T62" s="15"/>
     </row>
-    <row r="63" spans="6:20" ht="14.25" customHeight="1">
+    <row r="63" spans="1:20" ht="14.25" customHeight="1">
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
@@ -5491,7 +6489,7 @@
       <c r="S63" s="2"/>
       <c r="T63" s="15"/>
     </row>
-    <row r="64" spans="6:20" ht="14.25" customHeight="1">
+    <row r="64" spans="1:20" ht="14.25" customHeight="1">
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -13830,7 +14828,7 @@
       <c r="T607" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T28" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A9:T55" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:T28">
       <sortCondition ref="A9:A28"/>
     </sortState>
@@ -13879,10 +14877,10 @@
         <v>25</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -13890,13 +14888,13 @@
         <v>44</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -13904,13 +14902,13 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -13918,13 +14916,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -13932,13 +14930,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -13946,13 +14944,13 @@
         <v>50</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1">
@@ -13960,13 +14958,13 @@
         <v>51</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1">
@@ -13974,13 +14972,13 @@
         <v>52</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1">
@@ -13988,27 +14986,27 @@
         <v>53</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" hidden="1" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="C10" s="30">
         <v>191</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
@@ -14016,13 +15014,13 @@
         <v>44</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C11" s="30">
         <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14030,13 +15028,13 @@
         <v>47</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C12" s="30">
         <v>208</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14044,13 +15042,13 @@
         <v>48</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C13" s="30">
         <v>224</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>120</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14058,13 +15056,13 @@
         <v>49</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C14" s="30">
         <v>240</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14072,13 +15070,13 @@
         <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C15" s="30">
         <v>256</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14086,13 +15084,13 @@
         <v>51</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C16" s="30">
         <v>272</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14100,13 +15098,13 @@
         <v>52</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C17" s="30">
         <v>288</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" hidden="1" customHeight="1">
@@ -14114,13 +15112,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="C18" s="30">
         <v>304</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
@@ -14128,13 +15126,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C19" s="30">
         <v>193</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14142,13 +15140,13 @@
         <v>47</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C20" s="30">
         <v>209</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14156,13 +15154,13 @@
         <v>48</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C21" s="30">
         <v>225</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>129</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14170,13 +15168,13 @@
         <v>49</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C22" s="30">
         <v>241</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14184,13 +15182,13 @@
         <v>50</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C23" s="30">
         <v>257</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>131</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14198,13 +15196,13 @@
         <v>51</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C24" s="30">
         <v>273</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14212,13 +15210,13 @@
         <v>52</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C25" s="30">
         <v>289</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14226,13 +15224,13 @@
         <v>53</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="C26" s="30">
         <v>305</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
@@ -14240,13 +15238,13 @@
         <v>44</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C27" s="30">
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>136</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14254,13 +15252,13 @@
         <v>47</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C28" s="30">
         <v>210</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14268,13 +15266,13 @@
         <v>48</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C29" s="30">
         <v>226</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14282,13 +15280,13 @@
         <v>49</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C30" s="30">
         <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14296,13 +15294,13 @@
         <v>50</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C31" s="30">
         <v>258</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>140</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14310,13 +15308,13 @@
         <v>51</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C32" s="30">
         <v>274</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14324,13 +15322,13 @@
         <v>52</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C33" s="30">
         <v>290</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>142</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14338,13 +15336,13 @@
         <v>53</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C34" s="30">
         <v>306</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>143</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
@@ -14352,7 +15350,7 @@
         <v>44</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C35" s="30">
         <v>195</v>
@@ -14366,7 +15364,7 @@
         <v>47</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C36" s="30">
         <v>211</v>
@@ -14380,7 +15378,7 @@
         <v>48</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C37" s="30">
         <v>227</v>
@@ -14394,7 +15392,7 @@
         <v>49</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C38" s="30">
         <v>243</v>
@@ -14408,7 +15406,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C39" s="30">
         <v>259</v>
@@ -14422,7 +15420,7 @@
         <v>51</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C40" s="30">
         <v>275</v>
@@ -14436,7 +15434,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C41" s="30">
         <v>291</v>
@@ -14450,7 +15448,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C42" s="30">
         <v>307</v>
@@ -14464,7 +15462,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C43" s="30">
         <v>196</v>
@@ -14478,7 +15476,7 @@
         <v>47</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C44" s="30">
         <v>212</v>
@@ -14492,7 +15490,7 @@
         <v>48</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C45" s="30">
         <v>228</v>
@@ -14506,7 +15504,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C46" s="30">
         <v>244</v>
@@ -14520,7 +15518,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C47" s="30">
         <v>260</v>
@@ -14534,7 +15532,7 @@
         <v>51</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C48" s="30">
         <v>276</v>
@@ -14548,7 +15546,7 @@
         <v>52</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C49" s="30">
         <v>292</v>
@@ -14562,7 +15560,7 @@
         <v>53</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C50" s="30">
         <v>308</v>
@@ -15554,18 +16552,18 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
correzione data.json e checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sorgenti\FSE 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.morelli\Documents\GitHub\it-fse-accreditamento\GATEWAY\A1#111BOLLINOXXXX\BOLLINOITSPA\BOLLINOFSE\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3114A2B0-1EA5-43FA-AC78-117AA3DB1C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FF6582-E03B-4411-86F7-17B7190EDBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Summary!$A$1:$D$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$54</definedName>
     <definedName name="filtro" localSheetId="2">TestCases!$A$9:$S$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="261">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -729,15 +729,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Laboratorio dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST- OK" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
   </si>
   <si>
     <t>ID TEST CASE OK</t>
@@ -1557,7 +1548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1677,6 +1668,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1698,15 +1695,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4164,13 +4152,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T607"/>
+  <dimension ref="A1:T606"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L47" sqref="L47"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4212,14 +4200,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" s="46"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="48"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4237,14 +4225,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="54" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="56" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="48"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4262,12 +4250,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" s="46"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="48"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4286,12 +4274,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="54" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="46"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="48"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4309,8 +4297,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4447,13 +4435,13 @@
         <v>45014</v>
       </c>
       <c r="G10" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="I10" s="24" t="s">
         <v>201</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>203</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>81</v>
@@ -4491,13 +4479,13 @@
         <v>45014</v>
       </c>
       <c r="G11" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I11" s="24" t="s">
         <v>204</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>206</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>81</v>
@@ -4535,13 +4523,13 @@
         <v>45014</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>81</v>
@@ -4579,13 +4567,13 @@
         <v>45015</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>81</v>
@@ -4623,13 +4611,13 @@
         <v>45014</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H14" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="I14" s="24" t="s">
         <v>214</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>216</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>81</v>
@@ -4667,13 +4655,13 @@
         <v>45014</v>
       </c>
       <c r="G15" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="I15" s="24" t="s">
         <v>222</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>224</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>81</v>
@@ -4686,13 +4674,13 @@
         <v>81</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O15" s="34" t="s">
         <v>81</v>
       </c>
       <c r="P15" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
@@ -4721,16 +4709,16 @@
         <v>45014</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="34" t="s">
@@ -4740,13 +4728,13 @@
         <v>81</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O16" s="34" t="s">
         <v>81</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4784,7 +4772,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4814,10 +4802,10 @@
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -4852,10 +4840,10 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
@@ -4890,10 +4878,10 @@
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
       <c r="J20" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -4928,10 +4916,10 @@
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
       <c r="J21" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -4966,10 +4954,10 @@
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
       <c r="J22" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -5004,10 +4992,10 @@
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
       <c r="J23" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -5042,10 +5030,10 @@
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
       <c r="J24" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -5080,10 +5068,10 @@
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -5117,37 +5105,37 @@
         <v>45014</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H26" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="I26" s="24" t="s">
         <v>229</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>231</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>81</v>
       </c>
       <c r="K26" s="25"/>
       <c r="L26" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M26" s="25" t="s">
         <v>81</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="P26" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
       <c r="S26" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>46</v>
@@ -5174,10 +5162,10 @@
       <c r="H27" s="24"/>
       <c r="I27" s="24"/>
       <c r="J27" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
@@ -5211,89 +5199,89 @@
         <v>45015</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>81</v>
       </c>
       <c r="K28" s="25"/>
       <c r="L28" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M28" s="25" t="s">
         <v>81</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="26"/>
       <c r="S28" s="27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="T28" s="28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
-      <c r="A29" s="20">
-        <v>191</v>
-      </c>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="40">
+        <v>11</v>
+      </c>
+      <c r="B29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="21" t="s">
-        <v>44</v>
+      <c r="C29" s="38" t="s">
+        <v>48</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>143</v>
+        <v>65</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="F29" s="23">
-        <v>45014</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="J29" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="35">
+        <v>45020</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="J29" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="28" t="s">
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="42" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A30" s="40">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" s="38" t="s">
         <v>54</v>
@@ -5302,27 +5290,21 @@
         <v>48</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="35">
-        <v>45020</v>
-      </c>
-      <c r="G30" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="H30" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="I30" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K30" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="J30" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="K30" s="33"/>
       <c r="L30" s="33"/>
       <c r="M30" s="33"/>
       <c r="N30" s="33"/>
@@ -5337,7 +5319,7 @@
     </row>
     <row r="31" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A31" s="40">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B31" s="38" t="s">
         <v>54</v>
@@ -5346,20 +5328,20 @@
         <v>48</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F31" s="35"/>
       <c r="G31" s="36"/>
       <c r="H31" s="36"/>
       <c r="I31" s="36"/>
       <c r="J31" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L31" s="33"/>
       <c r="M31" s="33"/>
@@ -5375,7 +5357,7 @@
     </row>
     <row r="32" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A32" s="40">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B32" s="38" t="s">
         <v>54</v>
@@ -5384,20 +5366,20 @@
         <v>48</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F32" s="35"/>
       <c r="G32" s="36"/>
       <c r="H32" s="36"/>
       <c r="I32" s="36"/>
       <c r="J32" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L32" s="33"/>
       <c r="M32" s="33"/>
@@ -5413,7 +5395,7 @@
     </row>
     <row r="33" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A33" s="40">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B33" s="38" t="s">
         <v>54</v>
@@ -5422,36 +5404,52 @@
         <v>48</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="K33" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="37"/>
+        <v>242</v>
+      </c>
+      <c r="F33" s="23">
+        <v>45014</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="K33" s="25"/>
+      <c r="L33" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="M33" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="N33" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="O33" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="P33" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="27"/>
       <c r="T33" s="42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A34" s="40">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B34" s="38" t="s">
         <v>54</v>
@@ -5460,25 +5458,25 @@
         <v>48</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F34" s="23">
         <v>45014</v>
       </c>
       <c r="G34" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="I34" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="H34" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="I34" s="24" t="s">
-        <v>224</v>
-      </c>
       <c r="J34" s="25" t="s">
-        <v>81</v>
+        <v>238</v>
       </c>
       <c r="K34" s="25"/>
       <c r="L34" s="34" t="s">
@@ -5488,13 +5486,13 @@
         <v>81</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O34" s="34" t="s">
         <v>81</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5505,7 +5503,7 @@
     </row>
     <row r="35" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A35" s="40">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B35" s="38" t="s">
         <v>54</v>
@@ -5514,41 +5512,25 @@
         <v>48</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>245</v>
-      </c>
-      <c r="F35" s="23">
+        <v>80</v>
+      </c>
+      <c r="F35" s="35">
         <v>45014</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="33" t="s">
         <v>225</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="I35" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="J35" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="K35" s="25"/>
-      <c r="L35" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="M35" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="N35" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="O35" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="P35" s="33" t="s">
-        <v>227</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -5559,7 +5541,7 @@
     </row>
     <row r="36" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A36" s="40">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B36" s="38" t="s">
         <v>54</v>
@@ -5568,36 +5550,36 @@
         <v>48</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" s="35">
-        <v>45014</v>
-      </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="26"/>
-      <c r="S36" s="27"/>
+        <v>106</v>
+      </c>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="K36" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="37"/>
       <c r="T36" s="42" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A37" s="40">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B37" s="38" t="s">
         <v>54</v>
@@ -5606,20 +5588,20 @@
         <v>48</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
       <c r="I37" s="36"/>
       <c r="J37" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="33"/>
@@ -5635,7 +5617,7 @@
     </row>
     <row r="38" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A38" s="40">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B38" s="38" t="s">
         <v>54</v>
@@ -5644,20 +5626,20 @@
         <v>48</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
       <c r="I38" s="36"/>
       <c r="J38" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="33"/>
@@ -5673,7 +5655,7 @@
     </row>
     <row r="39" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A39" s="40">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B39" s="38" t="s">
         <v>54</v>
@@ -5682,20 +5664,20 @@
         <v>48</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E39" s="39" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
       <c r="I39" s="36"/>
       <c r="J39" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="K39" s="25" t="s">
-        <v>212</v>
+        <v>195</v>
+      </c>
+      <c r="K39" s="33" t="s">
+        <v>216</v>
       </c>
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
@@ -5711,7 +5693,7 @@
     </row>
     <row r="40" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A40" s="40">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" s="38" t="s">
         <v>54</v>
@@ -5720,20 +5702,20 @@
         <v>48</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
       <c r="I40" s="36"/>
       <c r="J40" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L40" s="33"/>
       <c r="M40" s="33"/>
@@ -5749,7 +5731,7 @@
     </row>
     <row r="41" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A41" s="40">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" s="38" t="s">
         <v>54</v>
@@ -5758,20 +5740,20 @@
         <v>48</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F41" s="35"/>
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
       <c r="I41" s="36"/>
       <c r="J41" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="K41" s="33" t="s">
-        <v>219</v>
+        <v>195</v>
+      </c>
+      <c r="K41" s="25" t="s">
+        <v>211</v>
       </c>
       <c r="L41" s="33"/>
       <c r="M41" s="33"/>
@@ -5787,7 +5769,7 @@
     </row>
     <row r="42" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A42" s="40">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" s="38" t="s">
         <v>54</v>
@@ -5796,36 +5778,54 @@
         <v>48</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
-      <c r="P42" s="33"/>
+        <v>118</v>
+      </c>
+      <c r="F42" s="35">
+        <v>45022</v>
+      </c>
+      <c r="G42" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="H42" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="J42" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K42" s="33"/>
+      <c r="L42" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="M42" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N42" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="O42" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="P42" s="25" t="s">
+        <v>260</v>
+      </c>
       <c r="Q42" s="33"/>
       <c r="R42" s="41"/>
-      <c r="S42" s="37"/>
+      <c r="S42" s="37" t="s">
+        <v>259</v>
+      </c>
       <c r="T42" s="42" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A43" s="40">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B43" s="38" t="s">
         <v>54</v>
@@ -5834,54 +5834,36 @@
         <v>48</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E43" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="F43" s="35">
-        <v>45022</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>260</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>258</v>
-      </c>
-      <c r="I43" s="36" t="s">
-        <v>259</v>
-      </c>
-      <c r="J43" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="K43" s="33"/>
-      <c r="L43" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="M43" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="N43" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="O43" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="P43" s="25" t="s">
-        <v>262</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K43" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
       <c r="Q43" s="33"/>
       <c r="R43" s="41"/>
-      <c r="S43" s="37" t="s">
-        <v>261</v>
-      </c>
+      <c r="S43" s="37"/>
       <c r="T43" s="42" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A44" s="40">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B44" s="38" t="s">
         <v>54</v>
@@ -5890,20 +5872,20 @@
         <v>48</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E44" s="39" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="36"/>
       <c r="H44" s="36"/>
       <c r="I44" s="36"/>
-      <c r="J44" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="K44" s="33" t="s">
-        <v>228</v>
+      <c r="J44" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="K44" s="25" t="s">
+        <v>218</v>
       </c>
       <c r="L44" s="33"/>
       <c r="M44" s="33"/>
@@ -5919,7 +5901,7 @@
     </row>
     <row r="45" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A45" s="40">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B45" s="38" t="s">
         <v>54</v>
@@ -5928,36 +5910,54 @@
         <v>48</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="F45" s="35"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="K45" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-      <c r="N45" s="33"/>
-      <c r="O45" s="33"/>
-      <c r="P45" s="33"/>
+        <v>124</v>
+      </c>
+      <c r="F45" s="35">
+        <v>45021</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="H45" s="43" t="s">
+        <v>252</v>
+      </c>
+      <c r="I45" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="J45" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K45" s="33"/>
+      <c r="L45" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="M45" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N45" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="O45" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="P45" s="25" t="s">
+        <v>241</v>
+      </c>
       <c r="Q45" s="33"/>
       <c r="R45" s="41"/>
-      <c r="S45" s="37"/>
+      <c r="S45" s="44" t="s">
+        <v>255</v>
+      </c>
       <c r="T45" s="42" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A46" s="40">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B46" s="38" t="s">
         <v>54</v>
@@ -5966,54 +5966,36 @@
         <v>48</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E46" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="F46" s="35">
-        <v>45021</v>
-      </c>
-      <c r="G46" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="H46" s="55" t="s">
-        <v>254</v>
-      </c>
-      <c r="I46" s="55" t="s">
-        <v>255</v>
-      </c>
-      <c r="J46" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="K46" s="33"/>
-      <c r="L46" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="M46" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="N46" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="O46" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="P46" s="25" t="s">
-        <v>243</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="K46" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="33"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="33"/>
       <c r="Q46" s="33"/>
       <c r="R46" s="41"/>
-      <c r="S46" s="57" t="s">
-        <v>257</v>
-      </c>
+      <c r="S46" s="37"/>
       <c r="T46" s="42" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A47" s="40">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B47" s="38" t="s">
         <v>54</v>
@@ -6022,20 +6004,20 @@
         <v>48</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E47" s="39" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F47" s="35"/>
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
       <c r="I47" s="36"/>
-      <c r="J47" s="25" t="s">
-        <v>197</v>
+      <c r="J47" s="33" t="s">
+        <v>195</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -6051,7 +6033,7 @@
     </row>
     <row r="48" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A48" s="40">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B48" s="38" t="s">
         <v>54</v>
@@ -6060,20 +6042,20 @@
         <v>48</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F48" s="35"/>
       <c r="G48" s="36"/>
       <c r="H48" s="36"/>
       <c r="I48" s="36"/>
       <c r="J48" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -6089,7 +6071,7 @@
     </row>
     <row r="49" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A49" s="40">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B49" s="38" t="s">
         <v>54</v>
@@ -6098,20 +6080,20 @@
         <v>48</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E49" s="39" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="36"/>
       <c r="H49" s="36"/>
       <c r="I49" s="36"/>
       <c r="J49" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="33"/>
@@ -6127,7 +6109,7 @@
     </row>
     <row r="50" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A50" s="40">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B50" s="38" t="s">
         <v>54</v>
@@ -6136,20 +6118,20 @@
         <v>48</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="36"/>
       <c r="H50" s="36"/>
       <c r="I50" s="36"/>
       <c r="J50" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
@@ -6165,7 +6147,7 @@
     </row>
     <row r="51" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A51" s="40">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B51" s="38" t="s">
         <v>54</v>
@@ -6174,20 +6156,20 @@
         <v>48</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E51" s="39" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="36"/>
       <c r="H51" s="36"/>
       <c r="I51" s="36"/>
       <c r="J51" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="33"/>
@@ -6203,7 +6185,7 @@
     </row>
     <row r="52" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A52" s="40">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B52" s="38" t="s">
         <v>54</v>
@@ -6212,20 +6194,20 @@
         <v>48</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F52" s="35"/>
       <c r="G52" s="36"/>
       <c r="H52" s="36"/>
       <c r="I52" s="36"/>
       <c r="J52" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L52" s="33"/>
       <c r="M52" s="33"/>
@@ -6241,7 +6223,7 @@
     </row>
     <row r="53" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A53" s="40">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B53" s="38" t="s">
         <v>54</v>
@@ -6250,20 +6232,20 @@
         <v>48</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F53" s="35"/>
       <c r="G53" s="36"/>
       <c r="H53" s="36"/>
       <c r="I53" s="36"/>
       <c r="J53" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L53" s="33"/>
       <c r="M53" s="33"/>
@@ -6277,9 +6259,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+    <row r="54" spans="1:20" ht="34.950000000000003" customHeight="1">
       <c r="A54" s="40">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B54" s="38" t="s">
         <v>54</v>
@@ -6288,20 +6270,20 @@
         <v>48</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F54" s="35"/>
       <c r="G54" s="36"/>
       <c r="H54" s="36"/>
       <c r="I54" s="36"/>
       <c r="J54" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K54" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L54" s="33"/>
       <c r="M54" s="33"/>
@@ -6315,43 +6297,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="34.950000000000003" customHeight="1">
-      <c r="A55" s="40">
-        <v>93</v>
-      </c>
-      <c r="B55" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D55" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="E55" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="F55" s="35"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="K55" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="L55" s="33"/>
-      <c r="M55" s="33"/>
-      <c r="N55" s="33"/>
-      <c r="O55" s="33"/>
-      <c r="P55" s="33"/>
-      <c r="Q55" s="33"/>
-      <c r="R55" s="41"/>
-      <c r="S55" s="37"/>
-      <c r="T55" s="42" t="s">
-        <v>46</v>
-      </c>
+    <row r="55" spans="1:20" ht="14.25" customHeight="1">
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="15"/>
     </row>
     <row r="56" spans="1:20" ht="14.25" customHeight="1">
       <c r="F56" s="12"/>
@@ -14616,21 +14577,7 @@
       <c r="T541" s="15"/>
     </row>
     <row r="542" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F542" s="12"/>
-      <c r="G542" s="12"/>
-      <c r="H542" s="12"/>
-      <c r="I542" s="12"/>
-      <c r="J542" s="13"/>
-      <c r="K542" s="13"/>
-      <c r="L542" s="13"/>
-      <c r="M542" s="13"/>
-      <c r="N542" s="13"/>
-      <c r="O542" s="13"/>
-      <c r="P542" s="13"/>
-      <c r="Q542" s="13"/>
-      <c r="R542" s="14"/>
-      <c r="S542" s="2"/>
-      <c r="T542" s="15"/>
+      <c r="T542" s="13"/>
     </row>
     <row r="543" spans="6:20" ht="14.25" customHeight="1">
       <c r="T543" s="13"/>
@@ -14824,11 +14771,8 @@
     <row r="606" spans="20:20" ht="14.25" customHeight="1">
       <c r="T606" s="13"/>
     </row>
-    <row r="607" spans="20:20" ht="14.25" customHeight="1">
-      <c r="T607" s="13"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A9:T55" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A9:T54" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:T28">
       <sortCondition ref="A9:A28"/>
     </sortState>
@@ -14877,10 +14821,10 @@
         <v>25</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -14888,13 +14832,13 @@
         <v>44</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>147</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14902,13 +14846,13 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14916,13 +14860,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14930,13 +14874,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -14944,13 +14888,13 @@
         <v>50</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1">
@@ -14958,13 +14902,13 @@
         <v>51</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1">
@@ -14972,13 +14916,13 @@
         <v>52</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1">
@@ -14986,27 +14930,27 @@
         <v>53</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" hidden="1" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" s="30">
         <v>191</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
@@ -15014,13 +14958,13 @@
         <v>44</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C11" s="30">
         <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15028,13 +14972,13 @@
         <v>47</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" s="30">
         <v>208</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15042,13 +14986,13 @@
         <v>48</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" s="30">
         <v>224</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15056,13 +15000,13 @@
         <v>49</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C14" s="30">
         <v>240</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15070,13 +15014,13 @@
         <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C15" s="30">
         <v>256</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15084,13 +15028,13 @@
         <v>51</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C16" s="30">
         <v>272</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15098,13 +15042,13 @@
         <v>52</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C17" s="30">
         <v>288</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" hidden="1" customHeight="1">
@@ -15112,13 +15056,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" s="30">
         <v>304</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
@@ -15126,13 +15070,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C19" s="30">
         <v>193</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15140,13 +15084,13 @@
         <v>47</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C20" s="30">
         <v>209</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15154,13 +15098,13 @@
         <v>48</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C21" s="30">
         <v>225</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15168,13 +15112,13 @@
         <v>49</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C22" s="30">
         <v>241</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15182,13 +15126,13 @@
         <v>50</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C23" s="30">
         <v>257</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15196,13 +15140,13 @@
         <v>51</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C24" s="30">
         <v>273</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15210,13 +15154,13 @@
         <v>52</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C25" s="30">
         <v>289</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15224,13 +15168,13 @@
         <v>53</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C26" s="30">
         <v>305</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
@@ -15238,13 +15182,13 @@
         <v>44</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27" s="30">
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15252,13 +15196,13 @@
         <v>47</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28" s="30">
         <v>210</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15266,13 +15210,13 @@
         <v>48</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C29" s="30">
         <v>226</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15280,13 +15224,13 @@
         <v>49</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C30" s="30">
         <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15294,13 +15238,13 @@
         <v>50</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C31" s="30">
         <v>258</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15308,13 +15252,13 @@
         <v>51</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C32" s="30">
         <v>274</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15322,13 +15266,13 @@
         <v>52</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C33" s="30">
         <v>290</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" hidden="1" customHeight="1">
@@ -15336,13 +15280,13 @@
         <v>53</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C34" s="30">
         <v>306</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
@@ -15350,7 +15294,7 @@
         <v>44</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C35" s="30">
         <v>195</v>
@@ -15364,7 +15308,7 @@
         <v>47</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C36" s="30">
         <v>211</v>
@@ -15378,7 +15322,7 @@
         <v>48</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C37" s="30">
         <v>227</v>
@@ -15392,7 +15336,7 @@
         <v>49</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C38" s="30">
         <v>243</v>
@@ -15406,7 +15350,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C39" s="30">
         <v>259</v>
@@ -15420,7 +15364,7 @@
         <v>51</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C40" s="30">
         <v>275</v>
@@ -15434,7 +15378,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C41" s="30">
         <v>291</v>
@@ -15448,7 +15392,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C42" s="30">
         <v>307</v>
@@ -15462,7 +15406,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C43" s="30">
         <v>196</v>
@@ -15476,7 +15420,7 @@
         <v>47</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C44" s="30">
         <v>212</v>
@@ -15490,7 +15434,7 @@
         <v>48</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C45" s="30">
         <v>228</v>
@@ -15504,7 +15448,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C46" s="30">
         <v>244</v>
@@ -15518,7 +15462,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C47" s="30">
         <v>260</v>
@@ -15532,7 +15476,7 @@
         <v>51</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C48" s="30">
         <v>276</v>
@@ -15546,7 +15490,7 @@
         <v>52</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C49" s="30">
         <v>292</v>
@@ -15560,7 +15504,7 @@
         <v>53</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C50" s="30">
         <v>308</v>
@@ -16552,7 +16496,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>81</v>
@@ -16560,10 +16504,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
aggiunti i test case di specialistica
subject_application_id: BOLLINOFSE
subject_application_vendor: BOLLINOITSPA
subject_application_version: 1.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.morelli\Documents\GitHub\it-fse-accreditamento\GATEWAY\A1#111BOLLINOXXXX\BOLLINOITSPA\BOLLINOFSE\1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.morelli\Documents\GitHub\it-fse-accreditamento-main_new\GATEWAY\A1#111BOLLINOXXXX\BOLLINOITSPA\BOLLINOFSE\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01876E44-C6E5-45D0-AAF1-0EFA75F59ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB29850-1F56-490E-86E9-82B6D39B0969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="325">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -966,6 +966,9 @@
   </si>
   <si>
     <t>f56936a5f6789044</t>
+  </si>
+  <si>
+    <t>Verrà mostrato sullo schermo un messaggio di errore che sarà inoltre memorizzzato in un file di log con tutte le dovute informazioni aggiuntive</t>
   </si>
   <si>
     <t>Il sistema prevede esclusivamente la possibilità di inserire un valore "Normale" o "Urgente"</t>
@@ -1210,21 +1213,265 @@
     <t>L'applicativo non gestisce le sezioni opzionali</t>
   </si>
   <si>
-    <t>Verrà mostrato sullo schermo un messaggio di errore che sarà inoltre memorizzato in un file di log con tutte le dovute informazioni aggiuntive. L'operazione di retry verrà eseguita manualmente attraverso un cruscotto riepilogativo.</t>
-  </si>
-  <si>
-    <t>Verrà mostrato sullo schermo un messaggio di errore che sarà inoltre memorizzato in un file di log con tutte le dovute informazioni aggiuntive. Il medico potrà produrre il documento ma per effettuare l'invio dovrà correggere le informazioni segnalate come errate</t>
+    <t>VALIDAZIONE_TOKEN_JWT_RSA_KO</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
+  </si>
+  <si>
+    <t>Verrà mostrato sullo schermo un messaggio di errore che sarà inoltre memorizzato in un file di log con tutte le dovute informazioni aggiuntive</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_RSA_TIMEOUT</t>
+  </si>
+  <si>
+    <t>Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
+"ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", "GESTIONE ERRORE".</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT7_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>In fase di inserimento anagrafica non è possibile immettere valori diversi da "maschio", "femmina" o "indifferenziato"</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-06-22T10:11:58Z</t>
+  </si>
+  <si>
+    <t>08be4f8281c6d7ff</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.8b53ea437c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Non è possibile produrre un referto senza averlo compilato</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Tutte le informazioni della sezione "Prestazioni" sono obbligatorie</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>Il sistema non prevede la possibilità di inserire un codice diverso da "S"</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>2023-06-21T14:35:47Z</t>
+  </si>
+  <si>
+    <t>64110cfc7e2e7532</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.c6309b9371^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="12">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1666,186 +1913,195 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4306,10 +4562,10 @@
   <dimension ref="A1:T606"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4718,13 +4974,13 @@
         <v>45015</v>
       </c>
       <c r="G13" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>228</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>227</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>81</v>
@@ -4767,7 +5023,7 @@
       <c r="H14" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="36" t="s">
         <v>214</v>
       </c>
       <c r="J14" s="25" t="s">
@@ -4810,7 +5066,7 @@
         <v>195</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -4853,7 +5109,7 @@
         <v>219</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K16" s="34" t="s">
         <v>81</v>
@@ -4863,13 +5119,13 @@
         <v>81</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O16" s="34" t="s">
         <v>81</v>
       </c>
       <c r="P16" s="33" t="s">
-        <v>262</v>
+        <v>222</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4909,7 +5165,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="33" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -5007,7 +5263,7 @@
       <c r="D20" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="39" t="s">
         <v>88</v>
       </c>
       <c r="F20" s="23"/>
@@ -5121,7 +5377,7 @@
       <c r="D23" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="39" t="s">
         <v>94</v>
       </c>
       <c r="F23" s="23"/>
@@ -5159,7 +5415,7 @@
       <c r="D24" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="39" t="s">
         <v>96</v>
       </c>
       <c r="F24" s="23"/>
@@ -5170,7 +5426,7 @@
         <v>195</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="25"/>
@@ -5242,13 +5498,13 @@
         <v>45014</v>
       </c>
       <c r="G26" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="H26" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="H26" s="24" t="s">
-        <v>223</v>
-      </c>
       <c r="I26" s="24" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>81</v>
@@ -5261,18 +5517,18 @@
         <v>81</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O26" s="25" t="s">
         <v>195</v>
       </c>
       <c r="P26" s="33" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
       <c r="S26" s="37" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>46</v>
@@ -5302,7 +5558,7 @@
         <v>195</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L27" s="34"/>
       <c r="M27" s="25"/>
@@ -5336,13 +5592,13 @@
         <v>45015</v>
       </c>
       <c r="G28" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="I28" s="24" t="s">
         <v>232</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>231</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>81</v>
@@ -5355,18 +5611,18 @@
         <v>81</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O28" s="25" t="s">
         <v>195</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="26"/>
       <c r="S28" s="27" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="T28" s="28" t="s">
         <v>46</v>
@@ -5392,13 +5648,13 @@
         <v>45020</v>
       </c>
       <c r="G29" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="I29" s="36" t="s">
         <v>243</v>
-      </c>
-      <c r="H29" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="I29" s="36" t="s">
-        <v>242</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>81</v>
@@ -5440,7 +5696,7 @@
         <v>195</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L30" s="34"/>
       <c r="M30" s="33"/>
@@ -5478,7 +5734,7 @@
         <v>195</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="33"/>
@@ -5516,7 +5772,7 @@
         <v>195</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="33"/>
@@ -5544,7 +5800,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
@@ -5554,7 +5810,7 @@
         <v>195</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
@@ -5582,7 +5838,7 @@
         <v>78</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F34" s="23">
         <v>45014</v>
@@ -5590,14 +5846,14 @@
       <c r="G34" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="H34" s="24" t="s">
+      <c r="H34" s="36" t="s">
         <v>221</v>
       </c>
       <c r="I34" s="24" t="s">
         <v>219</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K34" s="25"/>
       <c r="L34" s="34" t="s">
@@ -5607,13 +5863,13 @@
         <v>81</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O34" s="34" t="s">
         <v>81</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>262</v>
+        <v>222</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5653,7 +5909,7 @@
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
       <c r="P35" s="33" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -5910,13 +6166,13 @@
         <v>45022</v>
       </c>
       <c r="G42" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="H42" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="I42" s="36" t="s">
         <v>252</v>
-      </c>
-      <c r="H42" s="36" t="s">
-        <v>250</v>
-      </c>
-      <c r="I42" s="36" t="s">
-        <v>251</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>81</v>
@@ -5929,18 +6185,18 @@
         <v>81</v>
       </c>
       <c r="N42" s="25" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O42" s="25" t="s">
         <v>195</v>
       </c>
       <c r="P42" s="25" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="Q42" s="33"/>
       <c r="R42" s="41"/>
       <c r="S42" s="37" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="T42" s="42" t="s">
         <v>46</v>
@@ -5970,7 +6226,7 @@
         <v>195</v>
       </c>
       <c r="K43" s="33" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L43" s="33"/>
       <c r="M43" s="33"/>
@@ -6042,13 +6298,13 @@
         <v>45021</v>
       </c>
       <c r="G45" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="H45" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="I45" s="52" t="s">
         <v>248</v>
-      </c>
-      <c r="H45" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="I45" s="52" t="s">
-        <v>247</v>
       </c>
       <c r="J45" s="47" t="s">
         <v>81</v>
@@ -6061,18 +6317,18 @@
         <v>81</v>
       </c>
       <c r="N45" s="25" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>195</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Q45" s="33"/>
       <c r="R45" s="41"/>
       <c r="S45" s="43" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="T45" s="42" t="s">
         <v>46</v>
@@ -6102,7 +6358,7 @@
         <v>195</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>
@@ -6140,7 +6396,7 @@
         <v>195</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -6178,7 +6434,7 @@
         <v>195</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -6216,7 +6472,7 @@
         <v>195</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="33"/>
@@ -6230,7 +6486,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+    <row r="50" spans="1:20" ht="34.799999999999997" customHeight="1" thickBot="1">
       <c r="A50" s="40">
         <v>89</v>
       </c>
@@ -6254,7 +6510,7 @@
         <v>195</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
@@ -6292,7 +6548,7 @@
         <v>195</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L51" s="33"/>
       <c r="M51" s="33"/>
@@ -6330,7 +6586,7 @@
         <v>195</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L52" s="33"/>
       <c r="M52" s="33"/>
@@ -6344,7 +6600,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="34.950000000000003" customHeight="1" thickBot="1">
+    <row r="53" spans="1:20" ht="34.799999999999997" customHeight="1" thickBot="1">
       <c r="A53" s="40">
         <v>92</v>
       </c>
@@ -6368,7 +6624,7 @@
         <v>195</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L53" s="33"/>
       <c r="M53" s="33"/>
@@ -6406,7 +6662,7 @@
         <v>195</v>
       </c>
       <c r="K54" s="33" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L54" s="33"/>
       <c r="M54" s="33"/>
@@ -6420,7 +6676,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="30" customHeight="1">
+    <row r="55" spans="1:20" ht="30" customHeight="1" thickBot="1">
       <c r="A55" s="20">
         <v>191</v>
       </c>
@@ -6431,10 +6687,10 @@
         <v>44</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="24"/>
@@ -6444,7 +6700,7 @@
         <v>195</v>
       </c>
       <c r="K55" s="25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -6458,466 +6714,1054 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="13"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="13"/>
-      <c r="R56" s="14"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="15"/>
-    </row>
-    <row r="57" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
-      <c r="L57" s="13"/>
-      <c r="M57" s="13"/>
-      <c r="N57" s="13"/>
-      <c r="O57" s="13"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="13"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="15"/>
-    </row>
-    <row r="58" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="13"/>
-      <c r="L58" s="13"/>
-      <c r="M58" s="13"/>
-      <c r="N58" s="13"/>
-      <c r="O58" s="13"/>
-      <c r="P58" s="13"/>
-      <c r="Q58" s="13"/>
-      <c r="R58" s="14"/>
-      <c r="S58" s="2"/>
-      <c r="T58" s="15"/>
-    </row>
-    <row r="59" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="13"/>
-      <c r="N59" s="13"/>
-      <c r="O59" s="13"/>
-      <c r="P59" s="13"/>
-      <c r="Q59" s="13"/>
-      <c r="R59" s="14"/>
-      <c r="S59" s="2"/>
-      <c r="T59" s="15"/>
-    </row>
-    <row r="60" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="13"/>
-      <c r="K60" s="13"/>
-      <c r="L60" s="13"/>
-      <c r="M60" s="13"/>
-      <c r="N60" s="13"/>
-      <c r="O60" s="13"/>
-      <c r="P60" s="13"/>
-      <c r="Q60" s="13"/>
-      <c r="R60" s="14"/>
-      <c r="S60" s="2"/>
-      <c r="T60" s="15"/>
-    </row>
-    <row r="61" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
-      <c r="N61" s="13"/>
-      <c r="O61" s="13"/>
-      <c r="P61" s="13"/>
-      <c r="Q61" s="13"/>
-      <c r="R61" s="14"/>
-      <c r="S61" s="2"/>
-      <c r="T61" s="15"/>
-    </row>
-    <row r="62" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="13"/>
-      <c r="P62" s="13"/>
-      <c r="Q62" s="13"/>
-      <c r="R62" s="14"/>
-      <c r="S62" s="2"/>
-      <c r="T62" s="15"/>
-    </row>
-    <row r="63" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13"/>
-      <c r="O63" s="13"/>
-      <c r="P63" s="13"/>
-      <c r="Q63" s="13"/>
-      <c r="R63" s="14"/>
-      <c r="S63" s="2"/>
-      <c r="T63" s="15"/>
-    </row>
-    <row r="64" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13"/>
-      <c r="O64" s="13"/>
-      <c r="P64" s="13"/>
-      <c r="Q64" s="13"/>
-      <c r="R64" s="14"/>
-      <c r="S64" s="2"/>
-      <c r="T64" s="15"/>
-    </row>
-    <row r="65" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13"/>
-      <c r="O65" s="13"/>
-      <c r="P65" s="13"/>
-      <c r="Q65" s="13"/>
-      <c r="R65" s="14"/>
-      <c r="S65" s="2"/>
-      <c r="T65" s="15"/>
-    </row>
-    <row r="66" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="13"/>
-      <c r="P66" s="13"/>
-      <c r="Q66" s="13"/>
-      <c r="R66" s="14"/>
-      <c r="S66" s="2"/>
-      <c r="T66" s="15"/>
-    </row>
-    <row r="67" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="13"/>
-      <c r="R67" s="14"/>
-      <c r="S67" s="2"/>
-      <c r="T67" s="15"/>
-    </row>
-    <row r="68" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
-      <c r="P68" s="13"/>
-      <c r="Q68" s="13"/>
-      <c r="R68" s="14"/>
-      <c r="S68" s="2"/>
-      <c r="T68" s="15"/>
-    </row>
-    <row r="69" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13"/>
-      <c r="O69" s="13"/>
-      <c r="P69" s="13"/>
-      <c r="Q69" s="13"/>
-      <c r="R69" s="14"/>
-      <c r="S69" s="2"/>
-      <c r="T69" s="15"/>
-    </row>
-    <row r="70" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-      <c r="O70" s="13"/>
-      <c r="P70" s="13"/>
-      <c r="Q70" s="13"/>
-      <c r="R70" s="14"/>
-      <c r="S70" s="2"/>
-      <c r="T70" s="15"/>
-    </row>
-    <row r="71" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-      <c r="N71" s="13"/>
-      <c r="O71" s="13"/>
-      <c r="P71" s="13"/>
-      <c r="Q71" s="13"/>
-      <c r="R71" s="14"/>
-      <c r="S71" s="2"/>
-      <c r="T71" s="15"/>
-    </row>
-    <row r="72" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="13"/>
-      <c r="N72" s="13"/>
-      <c r="O72" s="13"/>
-      <c r="P72" s="13"/>
-      <c r="Q72" s="13"/>
-      <c r="R72" s="14"/>
-      <c r="S72" s="2"/>
-      <c r="T72" s="15"/>
-    </row>
-    <row r="73" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="13"/>
-      <c r="O73" s="13"/>
-      <c r="P73" s="13"/>
-      <c r="Q73" s="13"/>
-      <c r="R73" s="14"/>
-      <c r="S73" s="2"/>
-      <c r="T73" s="15"/>
-    </row>
-    <row r="74" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-      <c r="Q74" s="13"/>
-      <c r="R74" s="14"/>
-      <c r="S74" s="2"/>
-      <c r="T74" s="15"/>
-    </row>
-    <row r="75" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-      <c r="O75" s="13"/>
-      <c r="P75" s="13"/>
-      <c r="Q75" s="13"/>
-      <c r="R75" s="14"/>
-      <c r="S75" s="2"/>
-      <c r="T75" s="15"/>
-    </row>
-    <row r="76" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13"/>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="13"/>
-      <c r="R76" s="14"/>
-      <c r="S76" s="2"/>
-      <c r="T76" s="15"/>
-    </row>
-    <row r="77" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13"/>
-      <c r="P77" s="13"/>
-      <c r="Q77" s="13"/>
-      <c r="R77" s="14"/>
-      <c r="S77" s="2"/>
-      <c r="T77" s="15"/>
-    </row>
-    <row r="78" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="13"/>
-      <c r="P78" s="13"/>
-      <c r="Q78" s="13"/>
-      <c r="R78" s="14"/>
-      <c r="S78" s="2"/>
-      <c r="T78" s="15"/>
-    </row>
-    <row r="79" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="13"/>
-      <c r="N79" s="13"/>
-      <c r="O79" s="13"/>
-      <c r="P79" s="13"/>
-      <c r="Q79" s="13"/>
-      <c r="R79" s="14"/>
-      <c r="S79" s="2"/>
-      <c r="T79" s="15"/>
-    </row>
-    <row r="80" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="13"/>
-      <c r="R80" s="14"/>
-      <c r="S80" s="2"/>
-      <c r="T80" s="15"/>
-    </row>
-    <row r="81" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
-      <c r="O81" s="13"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="13"/>
-      <c r="R81" s="14"/>
-      <c r="S81" s="2"/>
-      <c r="T81" s="15"/>
-    </row>
-    <row r="82" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
-      <c r="O82" s="13"/>
-      <c r="P82" s="13"/>
-      <c r="Q82" s="13"/>
-      <c r="R82" s="14"/>
-      <c r="S82" s="2"/>
-      <c r="T82" s="15"/>
-    </row>
-    <row r="83" spans="6:20" ht="14.25" customHeight="1">
+    <row r="56" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A56" s="40">
+        <v>32</v>
+      </c>
+      <c r="B56" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="J56" s="68" t="s">
+        <v>195</v>
+      </c>
+      <c r="K56" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q56" s="33"/>
+      <c r="R56" s="41"/>
+      <c r="S56" s="37"/>
+      <c r="T56" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A57" s="40">
+        <v>40</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="F57" s="69">
+        <v>45014</v>
+      </c>
+      <c r="G57" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="H57" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="I57" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="J57" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K57" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="L57" s="33"/>
+      <c r="M57" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="N57" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="O57" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="P57" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q57" s="33"/>
+      <c r="R57" s="41"/>
+      <c r="S57" s="37"/>
+      <c r="T57" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A58" s="40">
+        <v>48</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="E58" s="39" t="s">
+        <v>266</v>
+      </c>
+      <c r="F58" s="69">
+        <v>45014</v>
+      </c>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="70"/>
+      <c r="J58" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K58" s="33"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="33"/>
+      <c r="N58" s="33"/>
+      <c r="O58" s="33"/>
+      <c r="P58" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q58" s="33"/>
+      <c r="R58" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="S58" s="37"/>
+      <c r="T58" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A59" s="40">
+        <v>147</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="E59" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="F59" s="69"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
+      <c r="J59" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K59" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="L59" s="33"/>
+      <c r="M59" s="33"/>
+      <c r="N59" s="33"/>
+      <c r="O59" s="33"/>
+      <c r="P59" s="33"/>
+      <c r="Q59" s="33"/>
+      <c r="R59" s="41"/>
+      <c r="S59" s="37"/>
+      <c r="T59" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A60" s="40">
+        <v>148</v>
+      </c>
+      <c r="B60" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="E60" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="F60" s="69"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
+      <c r="J60" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K60" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="L60" s="33"/>
+      <c r="M60" s="33"/>
+      <c r="N60" s="33"/>
+      <c r="O60" s="33"/>
+      <c r="P60" s="33"/>
+      <c r="Q60" s="33"/>
+      <c r="R60" s="41"/>
+      <c r="S60" s="37"/>
+      <c r="T60" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A61" s="40">
+        <v>149</v>
+      </c>
+      <c r="B61" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="E61" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="F61" s="69"/>
+      <c r="G61" s="70"/>
+      <c r="H61" s="70"/>
+      <c r="I61" s="70"/>
+      <c r="J61" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K61" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="N61" s="33"/>
+      <c r="O61" s="33"/>
+      <c r="P61" s="33"/>
+      <c r="Q61" s="33"/>
+      <c r="R61" s="41"/>
+      <c r="S61" s="37"/>
+      <c r="T61" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A62" s="40">
+        <v>150</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="E62" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="F62" s="69"/>
+      <c r="G62" s="70"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K62" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="L62" s="33"/>
+      <c r="M62" s="33"/>
+      <c r="N62" s="33"/>
+      <c r="O62" s="33"/>
+      <c r="P62" s="33"/>
+      <c r="Q62" s="33"/>
+      <c r="R62" s="41"/>
+      <c r="S62" s="37"/>
+      <c r="T62" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A63" s="40">
+        <v>151</v>
+      </c>
+      <c r="B63" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="E63" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="F63" s="69"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K63" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+      <c r="N63" s="33"/>
+      <c r="O63" s="33"/>
+      <c r="P63" s="33"/>
+      <c r="Q63" s="33"/>
+      <c r="R63" s="41"/>
+      <c r="S63" s="37"/>
+      <c r="T63" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A64" s="40">
+        <v>152</v>
+      </c>
+      <c r="B64" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="E64" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="F64" s="69"/>
+      <c r="G64" s="70"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K64" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+      <c r="N64" s="33"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="33"/>
+      <c r="Q64" s="33"/>
+      <c r="R64" s="41"/>
+      <c r="S64" s="37"/>
+      <c r="T64" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A65" s="40">
+        <v>153</v>
+      </c>
+      <c r="B65" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="E65" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="F65" s="69"/>
+      <c r="G65" s="70"/>
+      <c r="H65" s="70"/>
+      <c r="I65" s="70"/>
+      <c r="J65" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K65" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="33"/>
+      <c r="O65" s="33"/>
+      <c r="P65" s="33"/>
+      <c r="Q65" s="33"/>
+      <c r="R65" s="41"/>
+      <c r="S65" s="37"/>
+      <c r="T65" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A66" s="40">
+        <v>154</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="F66" s="69"/>
+      <c r="G66" s="70"/>
+      <c r="H66" s="70"/>
+      <c r="I66" s="70"/>
+      <c r="J66" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K66" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="L66" s="33"/>
+      <c r="M66" s="33"/>
+      <c r="N66" s="33"/>
+      <c r="O66" s="33"/>
+      <c r="P66" s="33"/>
+      <c r="Q66" s="33"/>
+      <c r="R66" s="41"/>
+      <c r="S66" s="37"/>
+      <c r="T66" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A67" s="40">
+        <v>155</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="F67" s="69"/>
+      <c r="G67" s="70"/>
+      <c r="H67" s="70"/>
+      <c r="I67" s="70"/>
+      <c r="J67" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K67" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="33"/>
+      <c r="O67" s="33"/>
+      <c r="P67" s="33"/>
+      <c r="Q67" s="33"/>
+      <c r="R67" s="41"/>
+      <c r="S67" s="37"/>
+      <c r="T67" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A68" s="40">
+        <v>156</v>
+      </c>
+      <c r="B68" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="F68" s="69"/>
+      <c r="G68" s="70"/>
+      <c r="H68" s="70"/>
+      <c r="I68" s="70"/>
+      <c r="J68" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K68" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="L68" s="33"/>
+      <c r="M68" s="33"/>
+      <c r="N68" s="33"/>
+      <c r="O68" s="33"/>
+      <c r="P68" s="33"/>
+      <c r="Q68" s="33"/>
+      <c r="R68" s="41"/>
+      <c r="S68" s="37"/>
+      <c r="T68" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A69" s="40">
+        <v>157</v>
+      </c>
+      <c r="B69" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>288</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="F69" s="69"/>
+      <c r="G69" s="70"/>
+      <c r="H69" s="70"/>
+      <c r="I69" s="70"/>
+      <c r="J69" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K69" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="L69" s="33"/>
+      <c r="M69" s="33"/>
+      <c r="N69" s="33"/>
+      <c r="O69" s="33"/>
+      <c r="P69" s="33"/>
+      <c r="Q69" s="33"/>
+      <c r="R69" s="41"/>
+      <c r="S69" s="37"/>
+      <c r="T69" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A70" s="40">
+        <v>158</v>
+      </c>
+      <c r="B70" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="38" t="s">
+        <v>290</v>
+      </c>
+      <c r="E70" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="F70" s="69"/>
+      <c r="G70" s="70"/>
+      <c r="H70" s="70"/>
+      <c r="I70" s="70"/>
+      <c r="J70" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K70" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="L70" s="33"/>
+      <c r="M70" s="33"/>
+      <c r="N70" s="33"/>
+      <c r="O70" s="33"/>
+      <c r="P70" s="33"/>
+      <c r="Q70" s="33"/>
+      <c r="R70" s="41"/>
+      <c r="S70" s="37"/>
+      <c r="T70" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A71" s="40">
+        <v>159</v>
+      </c>
+      <c r="B71" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C71" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="E71" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="F71" s="69"/>
+      <c r="G71" s="70"/>
+      <c r="H71" s="70"/>
+      <c r="I71" s="70"/>
+      <c r="J71" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="K71" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="L71" s="33"/>
+      <c r="M71" s="33"/>
+      <c r="N71" s="33"/>
+      <c r="O71" s="33"/>
+      <c r="P71" s="33"/>
+      <c r="Q71" s="33"/>
+      <c r="R71" s="41"/>
+      <c r="S71" s="37"/>
+      <c r="T71" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A72" s="40">
+        <v>160</v>
+      </c>
+      <c r="B72" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="E72" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="F72" s="69">
+        <v>45099</v>
+      </c>
+      <c r="G72" s="70" t="s">
+        <v>296</v>
+      </c>
+      <c r="H72" s="70" t="s">
+        <v>297</v>
+      </c>
+      <c r="I72" s="70" t="s">
+        <v>298</v>
+      </c>
+      <c r="J72" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K72" s="33"/>
+      <c r="L72" s="33"/>
+      <c r="M72" s="33"/>
+      <c r="N72" s="33"/>
+      <c r="O72" s="33"/>
+      <c r="P72" s="33"/>
+      <c r="Q72" s="33"/>
+      <c r="R72" s="41"/>
+      <c r="S72" s="37"/>
+      <c r="T72" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A73" s="40">
+        <v>161</v>
+      </c>
+      <c r="B73" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="E73" s="39" t="s">
+        <v>300</v>
+      </c>
+      <c r="F73" s="69"/>
+      <c r="G73" s="70"/>
+      <c r="H73" s="70"/>
+      <c r="I73" s="70"/>
+      <c r="J73" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K73" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="L73" s="33"/>
+      <c r="M73" s="33"/>
+      <c r="N73" s="33"/>
+      <c r="O73" s="33"/>
+      <c r="P73" s="33"/>
+      <c r="Q73" s="33"/>
+      <c r="R73" s="41"/>
+      <c r="S73" s="37"/>
+      <c r="T73" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A74" s="40">
+        <v>162</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E74" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="F74" s="69"/>
+      <c r="G74" s="70"/>
+      <c r="H74" s="70"/>
+      <c r="I74" s="70"/>
+      <c r="J74" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K74" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L74" s="33"/>
+      <c r="M74" s="33"/>
+      <c r="N74" s="33"/>
+      <c r="O74" s="33"/>
+      <c r="P74" s="33"/>
+      <c r="Q74" s="33"/>
+      <c r="R74" s="41"/>
+      <c r="S74" s="37"/>
+      <c r="T74" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A75" s="40">
+        <v>163</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="E75" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="F75" s="69"/>
+      <c r="G75" s="70"/>
+      <c r="H75" s="70"/>
+      <c r="I75" s="70"/>
+      <c r="J75" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K75" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="L75" s="33"/>
+      <c r="M75" s="33"/>
+      <c r="N75" s="33"/>
+      <c r="O75" s="33"/>
+      <c r="P75" s="33"/>
+      <c r="Q75" s="33"/>
+      <c r="R75" s="41"/>
+      <c r="S75" s="37"/>
+      <c r="T75" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A76" s="40">
+        <v>164</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C76" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="E76" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="F76" s="69"/>
+      <c r="G76" s="70"/>
+      <c r="H76" s="70"/>
+      <c r="I76" s="70"/>
+      <c r="J76" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K76" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L76" s="33"/>
+      <c r="M76" s="33"/>
+      <c r="N76" s="33"/>
+      <c r="O76" s="33"/>
+      <c r="P76" s="33"/>
+      <c r="Q76" s="33"/>
+      <c r="R76" s="41"/>
+      <c r="S76" s="37"/>
+      <c r="T76" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A77" s="40">
+        <v>165</v>
+      </c>
+      <c r="B77" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C77" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="E77" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="F77" s="69"/>
+      <c r="G77" s="70"/>
+      <c r="H77" s="70"/>
+      <c r="I77" s="70"/>
+      <c r="J77" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K77" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L77" s="33"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="33"/>
+      <c r="O77" s="33"/>
+      <c r="P77" s="33"/>
+      <c r="Q77" s="33"/>
+      <c r="R77" s="41"/>
+      <c r="S77" s="37"/>
+      <c r="T77" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A78" s="40">
+        <v>166</v>
+      </c>
+      <c r="B78" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D78" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="E78" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="F78" s="69"/>
+      <c r="G78" s="70"/>
+      <c r="H78" s="70"/>
+      <c r="I78" s="70"/>
+      <c r="J78" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K78" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L78" s="33"/>
+      <c r="M78" s="33"/>
+      <c r="N78" s="33"/>
+      <c r="O78" s="33"/>
+      <c r="P78" s="33"/>
+      <c r="Q78" s="33"/>
+      <c r="R78" s="41"/>
+      <c r="S78" s="37"/>
+      <c r="T78" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A79" s="40">
+        <v>167</v>
+      </c>
+      <c r="B79" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="E79" s="39" t="s">
+        <v>314</v>
+      </c>
+      <c r="F79" s="69"/>
+      <c r="G79" s="70"/>
+      <c r="H79" s="70"/>
+      <c r="I79" s="70"/>
+      <c r="J79" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K79" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L79" s="33"/>
+      <c r="M79" s="33"/>
+      <c r="N79" s="33"/>
+      <c r="O79" s="33"/>
+      <c r="P79" s="33"/>
+      <c r="Q79" s="33"/>
+      <c r="R79" s="41"/>
+      <c r="S79" s="37"/>
+      <c r="T79" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A80" s="40">
+        <v>168</v>
+      </c>
+      <c r="B80" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D80" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="E80" s="39" t="s">
+        <v>316</v>
+      </c>
+      <c r="F80" s="69"/>
+      <c r="G80" s="70"/>
+      <c r="H80" s="70"/>
+      <c r="I80" s="70"/>
+      <c r="J80" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="K80" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L80" s="33"/>
+      <c r="M80" s="33"/>
+      <c r="N80" s="33"/>
+      <c r="O80" s="33"/>
+      <c r="P80" s="33"/>
+      <c r="Q80" s="33"/>
+      <c r="R80" s="41"/>
+      <c r="S80" s="37"/>
+      <c r="T80" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" ht="35.4" customHeight="1" thickBot="1">
+      <c r="A81" s="40">
+        <v>169</v>
+      </c>
+      <c r="B81" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="E81" s="39" t="s">
+        <v>318</v>
+      </c>
+      <c r="F81" s="69"/>
+      <c r="G81" s="70"/>
+      <c r="H81" s="70"/>
+      <c r="I81" s="70"/>
+      <c r="J81" s="33"/>
+      <c r="K81" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="L81" s="33"/>
+      <c r="M81" s="33"/>
+      <c r="N81" s="33"/>
+      <c r="O81" s="33"/>
+      <c r="P81" s="33"/>
+      <c r="Q81" s="33"/>
+      <c r="R81" s="41"/>
+      <c r="S81" s="37"/>
+      <c r="T81" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" ht="35.4" customHeight="1">
+      <c r="A82" s="40">
+        <v>374</v>
+      </c>
+      <c r="B82" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="E82" s="39" t="s">
+        <v>321</v>
+      </c>
+      <c r="F82" s="69">
+        <v>45098</v>
+      </c>
+      <c r="G82" s="70" t="s">
+        <v>322</v>
+      </c>
+      <c r="H82" s="70" t="s">
+        <v>323</v>
+      </c>
+      <c r="I82" s="70" t="s">
+        <v>324</v>
+      </c>
+      <c r="J82" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="K82" s="33"/>
+      <c r="L82" s="33"/>
+      <c r="M82" s="33"/>
+      <c r="N82" s="33"/>
+      <c r="O82" s="33"/>
+      <c r="P82" s="33"/>
+      <c r="Q82" s="33"/>
+      <c r="R82" s="41"/>
+      <c r="S82" s="37"/>
+      <c r="T82" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" ht="14.25" customHeight="1">
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
@@ -6934,7 +7778,7 @@
       <c r="S83" s="2"/>
       <c r="T83" s="15"/>
     </row>
-    <row r="84" spans="6:20" ht="14.25" customHeight="1">
+    <row r="84" spans="1:20" ht="14.25" customHeight="1">
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
@@ -6951,7 +7795,7 @@
       <c r="S84" s="2"/>
       <c r="T84" s="15"/>
     </row>
-    <row r="85" spans="6:20" ht="14.25" customHeight="1">
+    <row r="85" spans="1:20" ht="14.25" customHeight="1">
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
@@ -6968,7 +7812,7 @@
       <c r="S85" s="2"/>
       <c r="T85" s="15"/>
     </row>
-    <row r="86" spans="6:20" ht="14.25" customHeight="1">
+    <row r="86" spans="1:20" ht="14.25" customHeight="1">
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
@@ -6985,7 +7829,7 @@
       <c r="S86" s="2"/>
       <c r="T86" s="15"/>
     </row>
-    <row r="87" spans="6:20" ht="14.25" customHeight="1">
+    <row r="87" spans="1:20" ht="14.25" customHeight="1">
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
@@ -7002,7 +7846,7 @@
       <c r="S87" s="2"/>
       <c r="T87" s="15"/>
     </row>
-    <row r="88" spans="6:20" ht="14.25" customHeight="1">
+    <row r="88" spans="1:20" ht="14.25" customHeight="1">
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
@@ -7019,7 +7863,7 @@
       <c r="S88" s="2"/>
       <c r="T88" s="15"/>
     </row>
-    <row r="89" spans="6:20" ht="14.25" customHeight="1">
+    <row r="89" spans="1:20" ht="14.25" customHeight="1">
       <c r="F89" s="12"/>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
@@ -7036,7 +7880,7 @@
       <c r="S89" s="2"/>
       <c r="T89" s="15"/>
     </row>
-    <row r="90" spans="6:20" ht="14.25" customHeight="1">
+    <row r="90" spans="1:20" ht="14.25" customHeight="1">
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
@@ -7053,7 +7897,7 @@
       <c r="S90" s="2"/>
       <c r="T90" s="15"/>
     </row>
-    <row r="91" spans="6:20" ht="14.25" customHeight="1">
+    <row r="91" spans="1:20" ht="14.25" customHeight="1">
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
@@ -7070,7 +7914,7 @@
       <c r="S91" s="2"/>
       <c r="T91" s="15"/>
     </row>
-    <row r="92" spans="6:20" ht="14.25" customHeight="1">
+    <row r="92" spans="1:20" ht="14.25" customHeight="1">
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
@@ -7087,7 +7931,7 @@
       <c r="S92" s="2"/>
       <c r="T92" s="15"/>
     </row>
-    <row r="93" spans="6:20" ht="14.25" customHeight="1">
+    <row r="93" spans="1:20" ht="14.25" customHeight="1">
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
@@ -7104,7 +7948,7 @@
       <c r="S93" s="2"/>
       <c r="T93" s="15"/>
     </row>
-    <row r="94" spans="6:20" ht="14.25" customHeight="1">
+    <row r="94" spans="1:20" ht="14.25" customHeight="1">
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
@@ -7121,7 +7965,7 @@
       <c r="S94" s="2"/>
       <c r="T94" s="15"/>
     </row>
-    <row r="95" spans="6:20" ht="14.25" customHeight="1">
+    <row r="95" spans="1:20" ht="14.25" customHeight="1">
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
@@ -7138,7 +7982,7 @@
       <c r="S95" s="2"/>
       <c r="T95" s="15"/>
     </row>
-    <row r="96" spans="6:20" ht="14.25" customHeight="1">
+    <row r="96" spans="1:20" ht="14.25" customHeight="1">
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>

</xml_diff>

<commit_message>
correzione checklist per accreditamento RSA
S1#111BOLLINOXXXX
BOLLINOITSPA
BOLLINOFSE
1.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.morelli\Documents\GitHub\it-fse-accreditamento-main_new\GATEWAY\A1#111BOLLINOXXXX\BOLLINOITSPA\BOLLINOFSE\1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.morelli\Documents\GitHub\it-fse-accreditamento\GATEWAY\A1#111BOLLINOXXXX\BOLLINOITSPA\BOLLINOFSE\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB29850-1F56-490E-86E9-82B6D39B0969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FC49CB-7387-4FAB-84DD-2EF886B4D6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="325">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2072,6 +2072,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2093,15 +2102,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4561,11 +4561,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T606"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4607,14 +4607,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="63" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="62"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4632,14 +4632,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="67" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="70" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="59"/>
+      <c r="D3" s="62"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4657,12 +4657,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="67" t="s">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="70" t="s">
         <v>197</v>
       </c>
-      <c r="D4" s="59"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4681,12 +4681,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="59"/>
+      <c r="D5" s="62"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4704,8 +4704,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="56"/>
-      <c r="B6" s="57"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -5111,9 +5111,7 @@
       <c r="J16" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="K16" s="34" t="s">
-        <v>81</v>
-      </c>
+      <c r="K16" s="34"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34" t="s">
         <v>81</v>
@@ -6730,7 +6728,7 @@
       <c r="E56" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="J56" s="68" t="s">
+      <c r="J56" s="56" t="s">
         <v>195</v>
       </c>
       <c r="K56" s="34" t="s">
@@ -6759,7 +6757,7 @@
       <c r="E57" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="F57" s="69">
+      <c r="F57" s="57">
         <v>45014</v>
       </c>
       <c r="G57" s="36" t="s">
@@ -6774,9 +6772,7 @@
       <c r="J57" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="K57" s="34" t="s">
-        <v>81</v>
-      </c>
+      <c r="K57" s="34"/>
       <c r="L57" s="33"/>
       <c r="M57" s="34" t="s">
         <v>81</v>
@@ -6813,12 +6809,12 @@
       <c r="E58" s="39" t="s">
         <v>266</v>
       </c>
-      <c r="F58" s="69">
+      <c r="F58" s="57">
         <v>45014</v>
       </c>
-      <c r="G58" s="70"/>
-      <c r="H58" s="70"/>
-      <c r="I58" s="70"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="58"/>
       <c r="J58" s="33" t="s">
         <v>81</v>
       </c>
@@ -6855,10 +6851,10 @@
       <c r="E59" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="F59" s="69"/>
-      <c r="G59" s="70"/>
-      <c r="H59" s="70"/>
-      <c r="I59" s="70"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="58"/>
       <c r="J59" s="33" t="s">
         <v>195</v>
       </c>
@@ -6893,10 +6889,10 @@
       <c r="E60" s="39" t="s">
         <v>270</v>
       </c>
-      <c r="F60" s="69"/>
-      <c r="G60" s="70"/>
-      <c r="H60" s="70"/>
-      <c r="I60" s="70"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
+      <c r="I60" s="58"/>
       <c r="J60" s="33" t="s">
         <v>195</v>
       </c>
@@ -6931,10 +6927,10 @@
       <c r="E61" s="39" t="s">
         <v>272</v>
       </c>
-      <c r="F61" s="69"/>
-      <c r="G61" s="70"/>
-      <c r="H61" s="70"/>
-      <c r="I61" s="70"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="58"/>
       <c r="J61" s="33" t="s">
         <v>195</v>
       </c>
@@ -6969,10 +6965,10 @@
       <c r="E62" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="F62" s="69"/>
-      <c r="G62" s="70"/>
-      <c r="H62" s="70"/>
-      <c r="I62" s="70"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="58"/>
+      <c r="I62" s="58"/>
       <c r="J62" s="33" t="s">
         <v>195</v>
       </c>
@@ -7007,10 +7003,10 @@
       <c r="E63" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="F63" s="69"/>
-      <c r="G63" s="70"/>
-      <c r="H63" s="70"/>
-      <c r="I63" s="70"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="58"/>
       <c r="J63" s="33" t="s">
         <v>195</v>
       </c>
@@ -7045,10 +7041,10 @@
       <c r="E64" s="39" t="s">
         <v>278</v>
       </c>
-      <c r="F64" s="69"/>
-      <c r="G64" s="70"/>
-      <c r="H64" s="70"/>
-      <c r="I64" s="70"/>
+      <c r="F64" s="57"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="58"/>
+      <c r="I64" s="58"/>
       <c r="J64" s="33" t="s">
         <v>195</v>
       </c>
@@ -7083,10 +7079,10 @@
       <c r="E65" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="F65" s="69"/>
-      <c r="G65" s="70"/>
-      <c r="H65" s="70"/>
-      <c r="I65" s="70"/>
+      <c r="F65" s="57"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
       <c r="J65" s="33" t="s">
         <v>195</v>
       </c>
@@ -7121,10 +7117,10 @@
       <c r="E66" s="39" t="s">
         <v>282</v>
       </c>
-      <c r="F66" s="69"/>
-      <c r="G66" s="70"/>
-      <c r="H66" s="70"/>
-      <c r="I66" s="70"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="58"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="58"/>
       <c r="J66" s="33" t="s">
         <v>195</v>
       </c>
@@ -7159,10 +7155,10 @@
       <c r="E67" s="39" t="s">
         <v>284</v>
       </c>
-      <c r="F67" s="69"/>
-      <c r="G67" s="70"/>
-      <c r="H67" s="70"/>
-      <c r="I67" s="70"/>
+      <c r="F67" s="57"/>
+      <c r="G67" s="58"/>
+      <c r="H67" s="58"/>
+      <c r="I67" s="58"/>
       <c r="J67" s="33" t="s">
         <v>195</v>
       </c>
@@ -7197,10 +7193,10 @@
       <c r="E68" s="39" t="s">
         <v>286</v>
       </c>
-      <c r="F68" s="69"/>
-      <c r="G68" s="70"/>
-      <c r="H68" s="70"/>
-      <c r="I68" s="70"/>
+      <c r="F68" s="57"/>
+      <c r="G68" s="58"/>
+      <c r="H68" s="58"/>
+      <c r="I68" s="58"/>
       <c r="J68" s="33" t="s">
         <v>195</v>
       </c>
@@ -7235,10 +7231,10 @@
       <c r="E69" s="39" t="s">
         <v>289</v>
       </c>
-      <c r="F69" s="69"/>
-      <c r="G69" s="70"/>
-      <c r="H69" s="70"/>
-      <c r="I69" s="70"/>
+      <c r="F69" s="57"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58"/>
+      <c r="I69" s="58"/>
       <c r="J69" s="33" t="s">
         <v>195</v>
       </c>
@@ -7273,10 +7269,10 @@
       <c r="E70" s="39" t="s">
         <v>291</v>
       </c>
-      <c r="F70" s="69"/>
-      <c r="G70" s="70"/>
-      <c r="H70" s="70"/>
-      <c r="I70" s="70"/>
+      <c r="F70" s="57"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="58"/>
       <c r="J70" s="33" t="s">
         <v>195</v>
       </c>
@@ -7311,10 +7307,10 @@
       <c r="E71" s="39" t="s">
         <v>293</v>
       </c>
-      <c r="F71" s="69"/>
-      <c r="G71" s="70"/>
-      <c r="H71" s="70"/>
-      <c r="I71" s="70"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
       <c r="J71" s="47" t="s">
         <v>195</v>
       </c>
@@ -7349,27 +7345,37 @@
       <c r="E72" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="F72" s="69">
+      <c r="F72" s="57">
         <v>45099</v>
       </c>
-      <c r="G72" s="70" t="s">
+      <c r="G72" s="58" t="s">
         <v>296</v>
       </c>
-      <c r="H72" s="70" t="s">
+      <c r="H72" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="I72" s="70" t="s">
+      <c r="I72" s="58" t="s">
         <v>298</v>
       </c>
       <c r="J72" s="33" t="s">
         <v>81</v>
       </c>
       <c r="K72" s="33"/>
-      <c r="L72" s="33"/>
-      <c r="M72" s="33"/>
-      <c r="N72" s="33"/>
-      <c r="O72" s="33"/>
-      <c r="P72" s="33"/>
+      <c r="L72" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="M72" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N72" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="O72" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="P72" s="25" t="s">
+        <v>238</v>
+      </c>
       <c r="Q72" s="33"/>
       <c r="R72" s="41"/>
       <c r="S72" s="37"/>
@@ -7393,10 +7399,10 @@
       <c r="E73" s="39" t="s">
         <v>300</v>
       </c>
-      <c r="F73" s="69"/>
-      <c r="G73" s="70"/>
-      <c r="H73" s="70"/>
-      <c r="I73" s="70"/>
+      <c r="F73" s="57"/>
+      <c r="G73" s="58"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="58"/>
       <c r="J73" s="33" t="s">
         <v>195</v>
       </c>
@@ -7431,10 +7437,10 @@
       <c r="E74" s="39" t="s">
         <v>303</v>
       </c>
-      <c r="F74" s="69"/>
-      <c r="G74" s="70"/>
-      <c r="H74" s="70"/>
-      <c r="I74" s="70"/>
+      <c r="F74" s="57"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
       <c r="J74" s="33" t="s">
         <v>195</v>
       </c>
@@ -7469,10 +7475,10 @@
       <c r="E75" s="39" t="s">
         <v>305</v>
       </c>
-      <c r="F75" s="69"/>
-      <c r="G75" s="70"/>
-      <c r="H75" s="70"/>
-      <c r="I75" s="70"/>
+      <c r="F75" s="57"/>
+      <c r="G75" s="58"/>
+      <c r="H75" s="58"/>
+      <c r="I75" s="58"/>
       <c r="J75" s="33" t="s">
         <v>195</v>
       </c>
@@ -7507,10 +7513,10 @@
       <c r="E76" s="39" t="s">
         <v>308</v>
       </c>
-      <c r="F76" s="69"/>
-      <c r="G76" s="70"/>
-      <c r="H76" s="70"/>
-      <c r="I76" s="70"/>
+      <c r="F76" s="57"/>
+      <c r="G76" s="58"/>
+      <c r="H76" s="58"/>
+      <c r="I76" s="58"/>
       <c r="J76" s="33" t="s">
         <v>195</v>
       </c>
@@ -7545,10 +7551,10 @@
       <c r="E77" s="39" t="s">
         <v>310</v>
       </c>
-      <c r="F77" s="69"/>
-      <c r="G77" s="70"/>
-      <c r="H77" s="70"/>
-      <c r="I77" s="70"/>
+      <c r="F77" s="57"/>
+      <c r="G77" s="58"/>
+      <c r="H77" s="58"/>
+      <c r="I77" s="58"/>
       <c r="J77" s="33" t="s">
         <v>195</v>
       </c>
@@ -7583,10 +7589,10 @@
       <c r="E78" s="39" t="s">
         <v>312</v>
       </c>
-      <c r="F78" s="69"/>
-      <c r="G78" s="70"/>
-      <c r="H78" s="70"/>
-      <c r="I78" s="70"/>
+      <c r="F78" s="57"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="58"/>
+      <c r="I78" s="58"/>
       <c r="J78" s="33" t="s">
         <v>195</v>
       </c>
@@ -7621,10 +7627,10 @@
       <c r="E79" s="39" t="s">
         <v>314</v>
       </c>
-      <c r="F79" s="69"/>
-      <c r="G79" s="70"/>
-      <c r="H79" s="70"/>
-      <c r="I79" s="70"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="58"/>
+      <c r="H79" s="58"/>
+      <c r="I79" s="58"/>
       <c r="J79" s="33" t="s">
         <v>195</v>
       </c>
@@ -7659,10 +7665,10 @@
       <c r="E80" s="39" t="s">
         <v>316</v>
       </c>
-      <c r="F80" s="69"/>
-      <c r="G80" s="70"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="70"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="58"/>
+      <c r="H80" s="58"/>
+      <c r="I80" s="58"/>
       <c r="J80" s="33" t="s">
         <v>195</v>
       </c>
@@ -7697,10 +7703,10 @@
       <c r="E81" s="39" t="s">
         <v>318</v>
       </c>
-      <c r="F81" s="69"/>
-      <c r="G81" s="70"/>
-      <c r="H81" s="70"/>
-      <c r="I81" s="70"/>
+      <c r="F81" s="57"/>
+      <c r="G81" s="58"/>
+      <c r="H81" s="58"/>
+      <c r="I81" s="58"/>
       <c r="J81" s="33"/>
       <c r="K81" s="33" t="s">
         <v>319</v>
@@ -7733,16 +7739,16 @@
       <c r="E82" s="39" t="s">
         <v>321</v>
       </c>
-      <c r="F82" s="69">
+      <c r="F82" s="57">
         <v>45098</v>
       </c>
-      <c r="G82" s="70" t="s">
+      <c r="G82" s="58" t="s">
         <v>322</v>
       </c>
-      <c r="H82" s="70" t="s">
+      <c r="H82" s="58" t="s">
         <v>323</v>
       </c>
-      <c r="I82" s="70" t="s">
+      <c r="I82" s="58" t="s">
         <v>324</v>
       </c>
       <c r="J82" s="33" t="s">

</xml_diff>

<commit_message>
correzione id 73, 169
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111BOLLINOXXXX/BOLLINOITSPA/BOLLINOFSE/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.morelli\Documents\GitHub\it-fse-accreditamento\GATEWAY\A1#111BOLLINOXXXX\BOLLINOITSPA\BOLLINOFSE\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CA1A10-C7E0-47D1-9962-0AEFD5347BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D79B9F1-38F1-448F-A068-7B63DB1A0C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Summary!$A$1:$D$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$105</definedName>
     <definedName name="filtro" localSheetId="2">TestCases!$A$9:$S$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="382">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -954,9 +954,6 @@
     "instance": "/validation/error",
     "workflowInstanceId": "2.16.840.1.113883.2.9.2.150.4.4.cce472283545a35052f3f7432f8d1334ac1d01c5c46f5a817ece8668b0083dbc.b0c96c8415^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"
 }</t>
-  </si>
-  <si>
-    <t>Si</t>
   </si>
   <si>
     <t>Impossibile invocare il servizio</t>
@@ -1664,6 +1661,9 @@
   </si>
   <si>
     <t>2023-07-25T12:10:35Z</t>
+  </si>
+  <si>
+    <t>L'operatore deve obbligatoriamente compilare i dati del Referto</t>
   </si>
 </sst>
 </file>
@@ -4776,11 +4776,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T606"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="D100" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="H55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F103" sqref="F103"/>
+      <selection pane="bottomRight" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -5057,13 +5057,13 @@
         <v>45128</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H10" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="I10" s="35" t="s">
         <v>334</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>335</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>81</v>
@@ -5101,13 +5101,13 @@
         <v>45128</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H11" s="35" t="s">
+        <v>336</v>
+      </c>
+      <c r="I11" s="35" t="s">
         <v>337</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>338</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>81</v>
@@ -5145,13 +5145,13 @@
         <v>45128</v>
       </c>
       <c r="G12" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="H12" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="I12" s="35" t="s">
         <v>341</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>342</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>81</v>
@@ -5189,13 +5189,13 @@
         <v>45128</v>
       </c>
       <c r="G13" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="H13" s="35" t="s">
         <v>343</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="I13" s="35" t="s">
         <v>344</v>
-      </c>
-      <c r="I13" s="35" t="s">
-        <v>345</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>81</v>
@@ -5233,13 +5233,13 @@
         <v>45128</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H14" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="I14" s="35" t="s">
         <v>346</v>
-      </c>
-      <c r="I14" s="35" t="s">
-        <v>347</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>81</v>
@@ -5281,7 +5281,7 @@
         <v>195</v>
       </c>
       <c r="K15" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L15" s="55"/>
       <c r="M15" s="55"/>
@@ -5315,10 +5315,10 @@
         <v>45127</v>
       </c>
       <c r="G16" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="H16" s="52" t="s">
         <v>327</v>
-      </c>
-      <c r="H16" s="52" t="s">
-        <v>328</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>207</v>
@@ -5334,13 +5334,13 @@
         <v>81</v>
       </c>
       <c r="N16" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O16" s="55" t="s">
         <v>81</v>
       </c>
       <c r="P16" s="55" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="Q16" s="55"/>
       <c r="R16" s="56"/>
@@ -5713,13 +5713,13 @@
         <v>45128</v>
       </c>
       <c r="G26" s="35" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H26" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="I26" s="35" t="s">
         <v>349</v>
-      </c>
-      <c r="I26" s="35" t="s">
-        <v>350</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>81</v>
@@ -5732,13 +5732,13 @@
         <v>81</v>
       </c>
       <c r="N26" s="55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O26" s="55" t="s">
         <v>195</v>
       </c>
       <c r="P26" s="55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q26" s="55"/>
       <c r="R26" s="56"/>
@@ -5773,7 +5773,7 @@
         <v>195</v>
       </c>
       <c r="K27" s="55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L27" s="55"/>
       <c r="M27" s="55"/>
@@ -5807,13 +5807,13 @@
         <v>45128</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H28" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="I28" s="35" t="s">
         <v>352</v>
-      </c>
-      <c r="I28" s="35" t="s">
-        <v>353</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>81</v>
@@ -5826,13 +5826,13 @@
         <v>81</v>
       </c>
       <c r="N28" s="55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O28" s="55" t="s">
         <v>195</v>
       </c>
       <c r="P28" s="55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q28" s="55"/>
       <c r="R28" s="56"/>
@@ -5863,13 +5863,13 @@
         <v>45128</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H29" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="I29" s="59" t="s">
         <v>355</v>
-      </c>
-      <c r="I29" s="59" t="s">
-        <v>356</v>
       </c>
       <c r="J29" s="55" t="s">
         <v>81</v>
@@ -5911,7 +5911,7 @@
         <v>195</v>
       </c>
       <c r="K30" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L30" s="55"/>
       <c r="M30" s="55"/>
@@ -5949,7 +5949,7 @@
         <v>195</v>
       </c>
       <c r="K31" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L31" s="55"/>
       <c r="M31" s="55"/>
@@ -5987,7 +5987,7 @@
         <v>195</v>
       </c>
       <c r="K32" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L32" s="55"/>
       <c r="M32" s="55"/>
@@ -6015,7 +6015,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
@@ -6025,7 +6025,7 @@
         <v>195</v>
       </c>
       <c r="K33" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L33" s="55"/>
       <c r="M33" s="55"/>
@@ -6053,22 +6053,22 @@
         <v>78</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F34" s="53">
         <v>45127</v>
       </c>
       <c r="G34" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="H34" s="52" t="s">
         <v>327</v>
-      </c>
-      <c r="H34" s="52" t="s">
-        <v>328</v>
       </c>
       <c r="I34" s="59" t="s">
         <v>207</v>
       </c>
       <c r="J34" s="55" t="s">
-        <v>212</v>
+        <v>81</v>
       </c>
       <c r="K34" s="55"/>
       <c r="L34" s="55" t="s">
@@ -6078,7 +6078,7 @@
         <v>81</v>
       </c>
       <c r="N34" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O34" s="55" t="s">
         <v>81</v>
@@ -6381,13 +6381,13 @@
         <v>45128</v>
       </c>
       <c r="G42" s="35" t="s">
+        <v>357</v>
+      </c>
+      <c r="H42" s="35" t="s">
         <v>358</v>
       </c>
-      <c r="H42" s="35" t="s">
+      <c r="I42" s="35" t="s">
         <v>359</v>
-      </c>
-      <c r="I42" s="35" t="s">
-        <v>360</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>81</v>
@@ -6400,18 +6400,18 @@
         <v>81</v>
       </c>
       <c r="N42" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O42" s="25" t="s">
         <v>195</v>
       </c>
       <c r="P42" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q42" s="33"/>
       <c r="R42" s="40"/>
       <c r="S42" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="T42" s="41" t="s">
         <v>46</v>
@@ -6513,13 +6513,13 @@
         <v>45128</v>
       </c>
       <c r="G45" s="35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H45" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="I45" s="58" t="s">
         <v>361</v>
-      </c>
-      <c r="I45" s="58" t="s">
-        <v>362</v>
       </c>
       <c r="J45" s="45" t="s">
         <v>81</v>
@@ -6532,18 +6532,18 @@
         <v>81</v>
       </c>
       <c r="N45" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>195</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q45" s="33"/>
       <c r="R45" s="40"/>
       <c r="S45" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T45" s="41" t="s">
         <v>46</v>
@@ -6573,7 +6573,7 @@
         <v>195</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>
@@ -6611,7 +6611,7 @@
         <v>195</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L47" s="33"/>
       <c r="M47" s="33"/>
@@ -6649,7 +6649,7 @@
         <v>195</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -6687,7 +6687,7 @@
         <v>195</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L49" s="33"/>
       <c r="M49" s="33"/>
@@ -6725,7 +6725,7 @@
         <v>195</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
@@ -6763,7 +6763,7 @@
         <v>195</v>
       </c>
       <c r="K51" s="55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L51" s="55"/>
       <c r="M51" s="55"/>
@@ -6801,7 +6801,7 @@
         <v>195</v>
       </c>
       <c r="K52" s="55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L52" s="55"/>
       <c r="M52" s="55"/>
@@ -6839,7 +6839,7 @@
         <v>195</v>
       </c>
       <c r="K53" s="55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L53" s="55"/>
       <c r="M53" s="55"/>
@@ -6877,7 +6877,7 @@
         <v>195</v>
       </c>
       <c r="K54" s="55" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L54" s="55"/>
       <c r="M54" s="55"/>
@@ -6902,10 +6902,10 @@
         <v>44</v>
       </c>
       <c r="D55" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>224</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>225</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="24"/>
@@ -6915,7 +6915,7 @@
         <v>195</v>
       </c>
       <c r="K55" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L55" s="55"/>
       <c r="M55" s="55"/>
@@ -6940,17 +6940,17 @@
         <v>52</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E56" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I56" s="60"/>
       <c r="J56" s="61" t="s">
         <v>195</v>
       </c>
       <c r="K56" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L56" s="60"/>
       <c r="M56" s="60"/>
@@ -6975,19 +6975,19 @@
         <v>52</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E57" s="38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F57" s="53">
         <v>45127</v>
       </c>
       <c r="G57" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="H57" s="52" t="s">
         <v>327</v>
-      </c>
-      <c r="H57" s="52" t="s">
-        <v>328</v>
       </c>
       <c r="I57" s="59" t="s">
         <v>207</v>
@@ -7003,13 +7003,13 @@
         <v>81</v>
       </c>
       <c r="N57" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O57" s="55" t="s">
         <v>81</v>
       </c>
       <c r="P57" s="55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q57" s="33"/>
       <c r="R57" s="40"/>
@@ -7029,10 +7029,10 @@
         <v>52</v>
       </c>
       <c r="D58" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="E58" s="38" t="s">
         <v>233</v>
-      </c>
-      <c r="E58" s="38" t="s">
-        <v>234</v>
       </c>
       <c r="F58" s="53">
         <v>45127</v>
@@ -7049,7 +7049,7 @@
       <c r="N58" s="55"/>
       <c r="O58" s="55"/>
       <c r="P58" s="55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q58" s="33"/>
       <c r="R58" s="40" t="s">
@@ -7071,10 +7071,10 @@
         <v>52</v>
       </c>
       <c r="D59" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="E59" s="38" t="s">
         <v>235</v>
-      </c>
-      <c r="E59" s="38" t="s">
-        <v>236</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="52"/>
@@ -7084,7 +7084,7 @@
         <v>195</v>
       </c>
       <c r="K59" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L59" s="55"/>
       <c r="M59" s="55"/>
@@ -7109,10 +7109,10 @@
         <v>52</v>
       </c>
       <c r="D60" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="E60" s="38" t="s">
         <v>237</v>
-      </c>
-      <c r="E60" s="38" t="s">
-        <v>238</v>
       </c>
       <c r="F60" s="51"/>
       <c r="G60" s="52"/>
@@ -7122,7 +7122,7 @@
         <v>195</v>
       </c>
       <c r="K60" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L60" s="33"/>
       <c r="M60" s="33"/>
@@ -7147,10 +7147,10 @@
         <v>52</v>
       </c>
       <c r="D61" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="E61" s="38" t="s">
         <v>239</v>
-      </c>
-      <c r="E61" s="38" t="s">
-        <v>240</v>
       </c>
       <c r="F61" s="51"/>
       <c r="G61" s="52"/>
@@ -7160,7 +7160,7 @@
         <v>195</v>
       </c>
       <c r="K61" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L61" s="33"/>
       <c r="M61" s="33"/>
@@ -7185,10 +7185,10 @@
         <v>52</v>
       </c>
       <c r="D62" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="E62" s="38" t="s">
         <v>241</v>
-      </c>
-      <c r="E62" s="38" t="s">
-        <v>242</v>
       </c>
       <c r="F62" s="51"/>
       <c r="G62" s="52"/>
@@ -7198,7 +7198,7 @@
         <v>195</v>
       </c>
       <c r="K62" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L62" s="33"/>
       <c r="M62" s="33"/>
@@ -7223,10 +7223,10 @@
         <v>52</v>
       </c>
       <c r="D63" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="E63" s="38" t="s">
         <v>243</v>
-      </c>
-      <c r="E63" s="38" t="s">
-        <v>244</v>
       </c>
       <c r="F63" s="51"/>
       <c r="G63" s="52"/>
@@ -7261,10 +7261,10 @@
         <v>52</v>
       </c>
       <c r="D64" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="E64" s="38" t="s">
         <v>245</v>
-      </c>
-      <c r="E64" s="38" t="s">
-        <v>246</v>
       </c>
       <c r="F64" s="51"/>
       <c r="G64" s="52"/>
@@ -7299,10 +7299,10 @@
         <v>52</v>
       </c>
       <c r="D65" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="E65" s="38" t="s">
         <v>247</v>
-      </c>
-      <c r="E65" s="38" t="s">
-        <v>248</v>
       </c>
       <c r="F65" s="51"/>
       <c r="G65" s="52"/>
@@ -7337,10 +7337,10 @@
         <v>52</v>
       </c>
       <c r="D66" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="E66" s="38" t="s">
         <v>249</v>
-      </c>
-      <c r="E66" s="38" t="s">
-        <v>250</v>
       </c>
       <c r="F66" s="51"/>
       <c r="G66" s="52"/>
@@ -7375,10 +7375,10 @@
         <v>52</v>
       </c>
       <c r="D67" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="E67" s="38" t="s">
         <v>251</v>
-      </c>
-      <c r="E67" s="38" t="s">
-        <v>252</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="52"/>
@@ -7413,10 +7413,10 @@
         <v>52</v>
       </c>
       <c r="D68" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="E68" s="38" t="s">
         <v>253</v>
-      </c>
-      <c r="E68" s="38" t="s">
-        <v>254</v>
       </c>
       <c r="F68" s="51"/>
       <c r="G68" s="52"/>
@@ -7426,7 +7426,7 @@
         <v>195</v>
       </c>
       <c r="K68" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L68" s="33"/>
       <c r="M68" s="33"/>
@@ -7451,10 +7451,10 @@
         <v>52</v>
       </c>
       <c r="D69" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="E69" s="38" t="s">
         <v>256</v>
-      </c>
-      <c r="E69" s="38" t="s">
-        <v>257</v>
       </c>
       <c r="F69" s="51"/>
       <c r="G69" s="52"/>
@@ -7464,7 +7464,7 @@
         <v>195</v>
       </c>
       <c r="K69" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L69" s="33"/>
       <c r="M69" s="33"/>
@@ -7489,10 +7489,10 @@
         <v>52</v>
       </c>
       <c r="D70" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="E70" s="38" t="s">
         <v>258</v>
-      </c>
-      <c r="E70" s="38" t="s">
-        <v>259</v>
       </c>
       <c r="F70" s="51"/>
       <c r="G70" s="52"/>
@@ -7527,10 +7527,10 @@
         <v>52</v>
       </c>
       <c r="D71" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="E71" s="38" t="s">
         <v>260</v>
-      </c>
-      <c r="E71" s="38" t="s">
-        <v>261</v>
       </c>
       <c r="F71" s="51"/>
       <c r="G71" s="52"/>
@@ -7565,22 +7565,22 @@
         <v>52</v>
       </c>
       <c r="D72" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="E72" s="38" t="s">
         <v>262</v>
-      </c>
-      <c r="E72" s="38" t="s">
-        <v>263</v>
       </c>
       <c r="F72" s="51">
         <v>45128</v>
       </c>
       <c r="G72" s="52" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H72" s="52" t="s">
+        <v>366</v>
+      </c>
+      <c r="I72" s="52" t="s">
         <v>367</v>
-      </c>
-      <c r="I72" s="52" t="s">
-        <v>368</v>
       </c>
       <c r="J72" s="33" t="s">
         <v>81</v>
@@ -7593,13 +7593,13 @@
         <v>81</v>
       </c>
       <c r="N72" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O72" s="25" t="s">
         <v>195</v>
       </c>
       <c r="P72" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q72" s="33"/>
       <c r="R72" s="40"/>
@@ -7619,10 +7619,10 @@
         <v>52</v>
       </c>
       <c r="D73" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="E73" s="38" t="s">
         <v>264</v>
-      </c>
-      <c r="E73" s="38" t="s">
-        <v>265</v>
       </c>
       <c r="F73" s="51"/>
       <c r="G73" s="52"/>
@@ -7632,7 +7632,7 @@
         <v>195</v>
       </c>
       <c r="K73" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L73" s="33"/>
       <c r="M73" s="33"/>
@@ -7657,10 +7657,10 @@
         <v>52</v>
       </c>
       <c r="D74" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="E74" s="38" t="s">
         <v>267</v>
-      </c>
-      <c r="E74" s="38" t="s">
-        <v>268</v>
       </c>
       <c r="F74" s="51"/>
       <c r="G74" s="52"/>
@@ -7670,7 +7670,7 @@
         <v>195</v>
       </c>
       <c r="K74" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L74" s="33"/>
       <c r="M74" s="33"/>
@@ -7695,10 +7695,10 @@
         <v>52</v>
       </c>
       <c r="D75" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E75" s="38" t="s">
         <v>269</v>
-      </c>
-      <c r="E75" s="38" t="s">
-        <v>270</v>
       </c>
       <c r="F75" s="51"/>
       <c r="G75" s="52"/>
@@ -7708,7 +7708,7 @@
         <v>195</v>
       </c>
       <c r="K75" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L75" s="33"/>
       <c r="M75" s="33"/>
@@ -7733,10 +7733,10 @@
         <v>52</v>
       </c>
       <c r="D76" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="E76" s="38" t="s">
         <v>272</v>
-      </c>
-      <c r="E76" s="38" t="s">
-        <v>273</v>
       </c>
       <c r="F76" s="51"/>
       <c r="G76" s="52"/>
@@ -7746,7 +7746,7 @@
         <v>195</v>
       </c>
       <c r="K76" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L76" s="33"/>
       <c r="M76" s="33"/>
@@ -7771,10 +7771,10 @@
         <v>52</v>
       </c>
       <c r="D77" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="E77" s="38" t="s">
         <v>274</v>
-      </c>
-      <c r="E77" s="38" t="s">
-        <v>275</v>
       </c>
       <c r="F77" s="51"/>
       <c r="G77" s="52"/>
@@ -7784,7 +7784,7 @@
         <v>195</v>
       </c>
       <c r="K77" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L77" s="33"/>
       <c r="M77" s="33"/>
@@ -7809,10 +7809,10 @@
         <v>52</v>
       </c>
       <c r="D78" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="E78" s="38" t="s">
         <v>276</v>
-      </c>
-      <c r="E78" s="38" t="s">
-        <v>277</v>
       </c>
       <c r="F78" s="51"/>
       <c r="G78" s="52"/>
@@ -7822,7 +7822,7 @@
         <v>195</v>
       </c>
       <c r="K78" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L78" s="33"/>
       <c r="M78" s="33"/>
@@ -7847,10 +7847,10 @@
         <v>52</v>
       </c>
       <c r="D79" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="E79" s="38" t="s">
         <v>278</v>
-      </c>
-      <c r="E79" s="38" t="s">
-        <v>279</v>
       </c>
       <c r="F79" s="51"/>
       <c r="G79" s="52"/>
@@ -7860,7 +7860,7 @@
         <v>195</v>
       </c>
       <c r="K79" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L79" s="33"/>
       <c r="M79" s="33"/>
@@ -7885,10 +7885,10 @@
         <v>52</v>
       </c>
       <c r="D80" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="E80" s="38" t="s">
         <v>280</v>
-      </c>
-      <c r="E80" s="38" t="s">
-        <v>281</v>
       </c>
       <c r="F80" s="51"/>
       <c r="G80" s="52"/>
@@ -7898,7 +7898,7 @@
         <v>195</v>
       </c>
       <c r="K80" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L80" s="33"/>
       <c r="M80" s="33"/>
@@ -7923,18 +7923,20 @@
         <v>52</v>
       </c>
       <c r="D81" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="E81" s="38" t="s">
         <v>282</v>
-      </c>
-      <c r="E81" s="38" t="s">
-        <v>283</v>
       </c>
       <c r="F81" s="51"/>
       <c r="G81" s="52"/>
       <c r="H81" s="52"/>
       <c r="I81" s="52"/>
-      <c r="J81" s="33"/>
+      <c r="J81" s="33" t="s">
+        <v>195</v>
+      </c>
       <c r="K81" s="33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L81" s="33"/>
       <c r="M81" s="33"/>
@@ -7959,22 +7961,22 @@
         <v>52</v>
       </c>
       <c r="D82" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="E82" s="38" t="s">
         <v>285</v>
-      </c>
-      <c r="E82" s="38" t="s">
-        <v>286</v>
       </c>
       <c r="F82" s="51">
         <v>45128</v>
       </c>
       <c r="G82" s="52" t="s">
+        <v>363</v>
+      </c>
+      <c r="H82" s="52" t="s">
         <v>364</v>
       </c>
-      <c r="H82" s="52" t="s">
+      <c r="I82" s="52" t="s">
         <v>365</v>
-      </c>
-      <c r="I82" s="52" t="s">
-        <v>366</v>
       </c>
       <c r="J82" s="33" t="s">
         <v>81</v>
@@ -8003,10 +8005,10 @@
         <v>47</v>
       </c>
       <c r="D83" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="E83" s="22" t="s">
         <v>287</v>
-      </c>
-      <c r="E83" s="22" t="s">
-        <v>288</v>
       </c>
       <c r="F83" s="51"/>
       <c r="G83" s="52"/>
@@ -8016,7 +8018,7 @@
         <v>195</v>
       </c>
       <c r="K83" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L83" s="55"/>
       <c r="M83" s="55"/>
@@ -8041,10 +8043,10 @@
         <v>47</v>
       </c>
       <c r="D84" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="E84" s="22" t="s">
         <v>289</v>
-      </c>
-      <c r="E84" s="22" t="s">
-        <v>290</v>
       </c>
       <c r="F84" s="51"/>
       <c r="G84" s="52"/>
@@ -8054,7 +8056,7 @@
         <v>195</v>
       </c>
       <c r="K84" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L84" s="55"/>
       <c r="M84" s="55"/>
@@ -8079,10 +8081,10 @@
         <v>47</v>
       </c>
       <c r="D85" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="E85" s="22" t="s">
         <v>291</v>
-      </c>
-      <c r="E85" s="22" t="s">
-        <v>292</v>
       </c>
       <c r="F85" s="51"/>
       <c r="G85" s="52"/>
@@ -8092,7 +8094,7 @@
         <v>195</v>
       </c>
       <c r="K85" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L85" s="55"/>
       <c r="M85" s="55"/>
@@ -8117,10 +8119,10 @@
         <v>47</v>
       </c>
       <c r="D86" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="E86" s="22" t="s">
         <v>293</v>
-      </c>
-      <c r="E86" s="22" t="s">
-        <v>294</v>
       </c>
       <c r="F86" s="51"/>
       <c r="G86" s="52"/>
@@ -8130,7 +8132,7 @@
         <v>195</v>
       </c>
       <c r="K86" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L86" s="55"/>
       <c r="M86" s="55"/>
@@ -8155,7 +8157,7 @@
         <v>47</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E87" s="22" t="s">
         <v>74</v>
@@ -8168,7 +8170,7 @@
         <v>195</v>
       </c>
       <c r="K87" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L87" s="55"/>
       <c r="M87" s="55"/>
@@ -8193,7 +8195,7 @@
         <v>47</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E88" s="38" t="s">
         <v>77</v>
@@ -8202,10 +8204,10 @@
         <v>45127</v>
       </c>
       <c r="G88" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="H88" s="52" t="s">
         <v>327</v>
-      </c>
-      <c r="H88" s="52" t="s">
-        <v>328</v>
       </c>
       <c r="I88" s="24" t="s">
         <v>207</v>
@@ -8221,7 +8223,7 @@
         <v>81</v>
       </c>
       <c r="N88" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O88" s="55" t="s">
         <v>81</v>
@@ -8247,10 +8249,10 @@
         <v>47</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E89" s="38" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F89" s="53">
         <v>45128</v>
@@ -8258,7 +8260,9 @@
       <c r="G89" s="54"/>
       <c r="H89" s="54"/>
       <c r="I89" s="54"/>
-      <c r="J89" s="25"/>
+      <c r="J89" s="25" t="s">
+        <v>81</v>
+      </c>
       <c r="K89" s="55"/>
       <c r="L89" s="55" t="s">
         <v>81</v>
@@ -8267,13 +8271,13 @@
         <v>81</v>
       </c>
       <c r="N89" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O89" s="55" t="s">
         <v>81</v>
       </c>
       <c r="P89" s="55" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="Q89" s="55"/>
       <c r="R89" s="56" t="s">
@@ -8295,10 +8299,10 @@
         <v>47</v>
       </c>
       <c r="D90" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="E90" s="38" t="s">
         <v>298</v>
-      </c>
-      <c r="E90" s="38" t="s">
-        <v>299</v>
       </c>
       <c r="F90" s="53"/>
       <c r="G90" s="54"/>
@@ -8333,10 +8337,10 @@
         <v>47</v>
       </c>
       <c r="D91" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="E91" s="22" t="s">
         <v>300</v>
-      </c>
-      <c r="E91" s="22" t="s">
-        <v>301</v>
       </c>
       <c r="F91" s="53"/>
       <c r="G91" s="54"/>
@@ -8371,10 +8375,10 @@
         <v>47</v>
       </c>
       <c r="D92" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E92" s="22" t="s">
         <v>302</v>
-      </c>
-      <c r="E92" s="22" t="s">
-        <v>303</v>
       </c>
       <c r="F92" s="53"/>
       <c r="G92" s="54"/>
@@ -8409,10 +8413,10 @@
         <v>47</v>
       </c>
       <c r="D93" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="E93" s="22" t="s">
         <v>304</v>
-      </c>
-      <c r="E93" s="22" t="s">
-        <v>305</v>
       </c>
       <c r="F93" s="53"/>
       <c r="G93" s="54"/>
@@ -8447,10 +8451,10 @@
         <v>47</v>
       </c>
       <c r="D94" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="E94" s="22" t="s">
         <v>306</v>
-      </c>
-      <c r="E94" s="22" t="s">
-        <v>307</v>
       </c>
       <c r="F94" s="53"/>
       <c r="G94" s="54"/>
@@ -8485,10 +8489,10 @@
         <v>47</v>
       </c>
       <c r="D95" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="E95" s="22" t="s">
         <v>308</v>
-      </c>
-      <c r="E95" s="22" t="s">
-        <v>309</v>
       </c>
       <c r="F95" s="53"/>
       <c r="G95" s="54"/>
@@ -8523,10 +8527,10 @@
         <v>47</v>
       </c>
       <c r="D96" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="E96" s="22" t="s">
         <v>310</v>
-      </c>
-      <c r="E96" s="22" t="s">
-        <v>311</v>
       </c>
       <c r="F96" s="53"/>
       <c r="G96" s="54"/>
@@ -8536,7 +8540,7 @@
         <v>195</v>
       </c>
       <c r="K96" s="55" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L96" s="55"/>
       <c r="M96" s="55"/>
@@ -8561,10 +8565,10 @@
         <v>47</v>
       </c>
       <c r="D97" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="E97" s="22" t="s">
         <v>312</v>
-      </c>
-      <c r="E97" s="22" t="s">
-        <v>313</v>
       </c>
       <c r="F97" s="53"/>
       <c r="G97" s="54"/>
@@ -8574,7 +8578,7 @@
         <v>195</v>
       </c>
       <c r="K97" s="55" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L97" s="55"/>
       <c r="M97" s="55"/>
@@ -8599,10 +8603,10 @@
         <v>47</v>
       </c>
       <c r="D98" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="E98" s="22" t="s">
         <v>314</v>
-      </c>
-      <c r="E98" s="22" t="s">
-        <v>315</v>
       </c>
       <c r="F98" s="53"/>
       <c r="G98" s="54"/>
@@ -8612,7 +8616,7 @@
         <v>195</v>
       </c>
       <c r="K98" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L98" s="55"/>
       <c r="M98" s="55"/>
@@ -8637,10 +8641,10 @@
         <v>47</v>
       </c>
       <c r="D99" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="E99" s="22" t="s">
         <v>316</v>
-      </c>
-      <c r="E99" s="22" t="s">
-        <v>317</v>
       </c>
       <c r="F99" s="53"/>
       <c r="G99" s="54"/>
@@ -8650,7 +8654,7 @@
         <v>195</v>
       </c>
       <c r="K99" s="55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L99" s="55"/>
       <c r="M99" s="55"/>
@@ -8675,32 +8679,42 @@
         <v>47</v>
       </c>
       <c r="D100" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="E100" s="38" t="s">
         <v>318</v>
-      </c>
-      <c r="E100" s="38" t="s">
-        <v>319</v>
       </c>
       <c r="F100" s="53">
         <v>45128</v>
       </c>
       <c r="G100" s="52" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H100" s="52" t="s">
+        <v>330</v>
+      </c>
+      <c r="I100" s="52" t="s">
         <v>331</v>
-      </c>
-      <c r="I100" s="52" t="s">
-        <v>332</v>
       </c>
       <c r="J100" s="33" t="s">
         <v>81</v>
       </c>
       <c r="K100" s="25"/>
-      <c r="L100" s="25"/>
-      <c r="M100" s="25"/>
-      <c r="N100" s="25"/>
-      <c r="O100" s="25"/>
-      <c r="P100" s="25"/>
+      <c r="L100" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="M100" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="N100" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="O100" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="P100" s="55" t="s">
+        <v>381</v>
+      </c>
       <c r="Q100" s="25"/>
       <c r="R100" s="26"/>
       <c r="S100" s="27"/>
@@ -8719,10 +8733,10 @@
         <v>47</v>
       </c>
       <c r="D101" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="E101" s="22" t="s">
         <v>320</v>
-      </c>
-      <c r="E101" s="22" t="s">
-        <v>321</v>
       </c>
       <c r="F101" s="53"/>
       <c r="G101" s="54"/>
@@ -8732,7 +8746,7 @@
         <v>195</v>
       </c>
       <c r="K101" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L101" s="25"/>
       <c r="M101" s="25"/>
@@ -8757,22 +8771,22 @@
         <v>47</v>
       </c>
       <c r="D102" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="E102" s="22" t="s">
         <v>322</v>
-      </c>
-      <c r="E102" s="22" t="s">
-        <v>323</v>
       </c>
       <c r="F102" s="53">
         <v>45127</v>
       </c>
       <c r="G102" s="52" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H102" s="52" t="s">
+        <v>323</v>
+      </c>
+      <c r="I102" s="52" t="s">
         <v>324</v>
-      </c>
-      <c r="I102" s="52" t="s">
-        <v>325</v>
       </c>
       <c r="J102" s="33" t="s">
         <v>81</v>
@@ -8801,22 +8815,22 @@
         <v>44</v>
       </c>
       <c r="D103" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="E103" s="22" t="s">
         <v>370</v>
-      </c>
-      <c r="E103" s="22" t="s">
-        <v>371</v>
       </c>
       <c r="F103" s="53">
         <v>45132</v>
       </c>
       <c r="G103" s="52" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H103" s="54" t="s">
+        <v>375</v>
+      </c>
+      <c r="I103" s="54" t="s">
         <v>376</v>
-      </c>
-      <c r="I103" s="54" t="s">
-        <v>377</v>
       </c>
       <c r="J103" s="25" t="s">
         <v>81</v>
@@ -8845,22 +8859,22 @@
         <v>48</v>
       </c>
       <c r="D104" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="E104" s="22" t="s">
         <v>372</v>
-      </c>
-      <c r="E104" s="22" t="s">
-        <v>373</v>
       </c>
       <c r="F104" s="53">
         <v>45132</v>
       </c>
       <c r="G104" s="52" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H104" s="54" t="s">
+        <v>378</v>
+      </c>
+      <c r="I104" s="54" t="s">
         <v>379</v>
-      </c>
-      <c r="I104" s="54" t="s">
-        <v>380</v>
       </c>
       <c r="J104" s="25" t="s">
         <v>81</v>
@@ -8889,10 +8903,10 @@
         <v>44</v>
       </c>
       <c r="D105" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="E105" s="22" t="s">
         <v>374</v>
-      </c>
-      <c r="E105" s="22" t="s">
-        <v>375</v>
       </c>
       <c r="F105" s="53"/>
       <c r="G105" s="54"/>
@@ -8902,7 +8916,7 @@
         <v>195</v>
       </c>
       <c r="K105" s="55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L105" s="25"/>
       <c r="M105" s="25"/>
@@ -16524,7 +16538,7 @@
       <c r="T606" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T102" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:T105" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>